<commit_message>
updated some of the protections
</commit_message>
<xml_diff>
--- a/league template.xlsx
+++ b/league template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goftaps-my.sharepoint.com/personal/sstaley_gofullthrottle_com/Documents/excel stuff/leagues/League-Points-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="647" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B7799E-6B35-47DD-A36C-576CD1682EF2}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2945338F-C519-4FB1-8B63-58A8A1DCC642}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="3" r:id="rId1"/>
-    <sheet name="Leaderboard 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Leaderboards" sheetId="1" r:id="rId2"/>
     <sheet name="Points calculator" sheetId="2" r:id="rId3"/>
     <sheet name="Juniors" sheetId="9" r:id="rId4"/>
     <sheet name="Division 1" sheetId="4" r:id="rId5"/>
@@ -2776,6 +2776,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}" name="leaderboard_division1" displayName="leaderboard_division1" ref="A3:J15" totalsRowShown="0" headerRowDxfId="240" dataDxfId="239">
   <autoFilter ref="A3:J15" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J15">
+    <sortCondition descending="1" ref="J3:J15"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3EE385B5-186A-494C-99F2-4DA44BADE713}" name="Name" dataDxfId="238">
       <calculatedColumnFormula>CONCATENATE(Roster!A4, " ", Roster!B4)</calculatedColumnFormula>
@@ -2815,6 +2818,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}" name="leaderboard_division2" displayName="leaderboard_division2" ref="A20:J32" totalsRowShown="0" headerRowDxfId="228" dataDxfId="227">
   <autoFilter ref="A20:J32" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:J32">
+    <sortCondition descending="1" ref="J20:J32"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{8920F168-081D-48F4-B861-3BF464DCB24E}" name="Name" dataDxfId="226">
       <calculatedColumnFormula>CONCATENATE(Roster!E4, " ", Roster!F4)</calculatedColumnFormula>
@@ -2854,6 +2860,9 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}" name="leaderboard_division3" displayName="leaderboard_division3" ref="M3:V15" totalsRowShown="0" headerRowDxfId="216" dataDxfId="215">
   <autoFilter ref="M3:V15" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:V15">
+    <sortCondition descending="1" ref="V3:V15"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{24729B62-D12C-44C0-A782-2B723A80950C}" name="Name" dataDxfId="214">
       <calculatedColumnFormula>CONCATENATE(roster_division3[[#This Row],[First Name]], " ", roster_division3[[#This Row],[Last Name]])</calculatedColumnFormula>
@@ -2893,6 +2902,9 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}" name="leaderboard_division0" displayName="leaderboard_division0" ref="M20:V32" totalsRowShown="0" headerRowDxfId="204" dataDxfId="203">
   <autoFilter ref="M20:V32" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M21:V32">
+    <sortCondition descending="1" ref="V20:V32"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{F5489658-A403-4D4D-8477-63F70A31236F}" name="Name" dataDxfId="202">
       <calculatedColumnFormula>CONCATENATE(Roster!M4, " ", Roster!N4)</calculatedColumnFormula>
@@ -3208,8 +3220,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3680,7 +3692,7 @@
   </sheetPr>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:J19"/>
     </sheetView>
   </sheetViews>
@@ -3919,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J15" si="0">SUM(B5:I5) - MIN(B5:I5)</f>
+        <f>SUM(B5:I5) - MIN(B5:I5)</f>
         <v>0</v>
       </c>
       <c r="M5" t="str">
@@ -3959,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:V15" si="1">SUM(N5:U5) - MIN(N5:U5)</f>
+        <f>SUM(N5:U5) - MIN(N5:U5)</f>
         <v>0</v>
       </c>
     </row>
@@ -4001,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f>SUM(B6:I6) - MIN(B6:I6)</f>
         <v>0</v>
       </c>
       <c r="M6" t="str">
@@ -4041,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
+        <f>SUM(N6:U6) - MIN(N6:U6)</f>
         <v>0</v>
       </c>
     </row>
@@ -4083,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f>SUM(B7:I7) - MIN(B7:I7)</f>
         <v>0</v>
       </c>
       <c r="M7" t="str">
@@ -4123,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
+        <f>SUM(N7:U7) - MIN(N7:U7)</f>
         <v>0</v>
       </c>
     </row>
@@ -4165,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f>SUM(B8:I8) - MIN(B8:I8)</f>
         <v>0</v>
       </c>
       <c r="M8" t="str">
@@ -4205,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
+        <f>SUM(N8:U8) - MIN(N8:U8)</f>
         <v>0</v>
       </c>
     </row>
@@ -4247,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f>SUM(B9:I9) - MIN(B9:I9)</f>
         <v>0</v>
       </c>
       <c r="M9" t="str">
@@ -4287,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
+        <f>SUM(N9:U9) - MIN(N9:U9)</f>
         <v>0</v>
       </c>
     </row>
@@ -4329,7 +4341,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f>SUM(B10:I10) - MIN(B10:I10)</f>
         <v>0</v>
       </c>
       <c r="M10" t="str">
@@ -4369,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
+        <f>SUM(N10:U10) - MIN(N10:U10)</f>
         <v>0</v>
       </c>
     </row>
@@ -4411,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f>SUM(B11:I11) - MIN(B11:I11)</f>
         <v>0</v>
       </c>
       <c r="M11" t="str">
@@ -4451,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
+        <f>SUM(N11:U11) - MIN(N11:U11)</f>
         <v>0</v>
       </c>
     </row>
@@ -4493,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f>SUM(B12:I12) - MIN(B12:I12)</f>
         <v>0</v>
       </c>
       <c r="M12" t="str">
@@ -4533,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
+        <f>SUM(N12:U12) - MIN(N12:U12)</f>
         <v>0</v>
       </c>
     </row>
@@ -4575,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f>SUM(B13:I13) - MIN(B13:I13)</f>
         <v>0</v>
       </c>
       <c r="M13" t="str">
@@ -4615,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f>SUM(N13:U13) - MIN(N13:U13)</f>
         <v>0</v>
       </c>
     </row>
@@ -4657,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f>SUM(B14:I14) - MIN(B14:I14)</f>
         <v>0</v>
       </c>
       <c r="M14" t="str">
@@ -4697,7 +4709,7 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
+        <f>SUM(N14:U14) - MIN(N14:U14)</f>
         <v>0</v>
       </c>
     </row>
@@ -4739,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f>SUM(B15:I15) - MIN(B15:I15)</f>
         <v>0</v>
       </c>
       <c r="M15" t="str">
@@ -4779,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="1"/>
+        <f>SUM(N15:U15) - MIN(N15:U15)</f>
         <v>0</v>
       </c>
     </row>
@@ -5029,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22:J32" si="2">SUM(B22:I22) - MIN(B22:I22)</f>
+        <f>SUM(B22:I22) - MIN(B22:I22)</f>
         <v>0</v>
       </c>
       <c r="M22" t="str">
@@ -5069,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:V32" si="3">SUM(N22:U22) - MIN(N22:U22)</f>
+        <f>SUM(N22:U22) - MIN(N22:U22)</f>
         <v>0</v>
       </c>
     </row>
@@ -5111,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
+        <f>SUM(B23:I23) - MIN(B23:I23)</f>
         <v>0</v>
       </c>
       <c r="M23" t="str">
@@ -5151,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <f t="shared" si="3"/>
+        <f>SUM(N23:U23) - MIN(N23:U23)</f>
         <v>0</v>
       </c>
     </row>
@@ -5193,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" si="2"/>
+        <f>SUM(B24:I24) - MIN(B24:I24)</f>
         <v>0</v>
       </c>
       <c r="M24" t="str">
@@ -5233,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="V24">
-        <f t="shared" si="3"/>
+        <f>SUM(N24:U24) - MIN(N24:U24)</f>
         <v>0</v>
       </c>
     </row>
@@ -5275,7 +5287,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <f t="shared" si="2"/>
+        <f>SUM(B25:I25) - MIN(B25:I25)</f>
         <v>0</v>
       </c>
       <c r="M25" t="str">
@@ -5315,7 +5327,7 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <f t="shared" si="3"/>
+        <f>SUM(N25:U25) - MIN(N25:U25)</f>
         <v>0</v>
       </c>
     </row>
@@ -5357,7 +5369,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f t="shared" si="2"/>
+        <f>SUM(B26:I26) - MIN(B26:I26)</f>
         <v>0</v>
       </c>
       <c r="M26" t="str">
@@ -5397,7 +5409,7 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <f t="shared" si="3"/>
+        <f>SUM(N26:U26) - MIN(N26:U26)</f>
         <v>0</v>
       </c>
     </row>
@@ -5439,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <f t="shared" si="2"/>
+        <f>SUM(B27:I27) - MIN(B27:I27)</f>
         <v>0</v>
       </c>
       <c r="M27" t="str">
@@ -5479,7 +5491,7 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <f t="shared" si="3"/>
+        <f>SUM(N27:U27) - MIN(N27:U27)</f>
         <v>0</v>
       </c>
     </row>
@@ -5521,7 +5533,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <f t="shared" si="2"/>
+        <f>SUM(B28:I28) - MIN(B28:I28)</f>
         <v>0</v>
       </c>
       <c r="M28" t="str">
@@ -5561,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="V28">
-        <f t="shared" si="3"/>
+        <f>SUM(N28:U28) - MIN(N28:U28)</f>
         <v>0</v>
       </c>
     </row>
@@ -5603,7 +5615,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <f t="shared" si="2"/>
+        <f>SUM(B29:I29) - MIN(B29:I29)</f>
         <v>0</v>
       </c>
       <c r="M29" t="str">
@@ -5643,7 +5655,7 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <f t="shared" si="3"/>
+        <f>SUM(N29:U29) - MIN(N29:U29)</f>
         <v>0</v>
       </c>
     </row>
@@ -5685,7 +5697,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <f t="shared" si="2"/>
+        <f>SUM(B30:I30) - MIN(B30:I30)</f>
         <v>0</v>
       </c>
       <c r="M30" t="str">
@@ -5725,7 +5737,7 @@
         <v>0</v>
       </c>
       <c r="V30">
-        <f t="shared" si="3"/>
+        <f>SUM(N30:U30) - MIN(N30:U30)</f>
         <v>0</v>
       </c>
     </row>
@@ -5767,7 +5779,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <f t="shared" si="2"/>
+        <f>SUM(B31:I31) - MIN(B31:I31)</f>
         <v>0</v>
       </c>
       <c r="M31" t="str">
@@ -5807,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" si="3"/>
+        <f>SUM(N31:U31) - MIN(N31:U31)</f>
         <v>0</v>
       </c>
     </row>
@@ -5849,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <f t="shared" si="2"/>
+        <f>SUM(B32:I32) - MIN(B32:I32)</f>
         <v>0</v>
       </c>
       <c r="M32" t="str">
@@ -5889,12 +5901,12 @@
         <v>0</v>
       </c>
       <c r="V32">
-        <f t="shared" si="3"/>
+        <f>SUM(N32:U32) - MIN(N32:U32)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aZ85sTYbCyCasgRF+E4UH+Ibjd34/r5SVgqsWGgHFzgKXY2Igky95P4vxiLvIRQbvxQCc1U9TlY76y+cSbZWTg==" saltValue="SW+fzcYyEjxDjUo5BOpsMA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2ZlPNzdv9/FOfufX/BQkDfTY7y1cHQLD676bl+mOgDCxqPs+rIwovvrWp8mZY11xonvZJX8pkwHFOEOdmAIwVg==" saltValue="Lls+mKvTD7ZyjUHPyNW6Kw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="5">
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="A18:J19"/>
@@ -5932,8 +5944,8 @@
   </sheetPr>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="C45" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6116,7 +6128,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="26" t="str">
-        <f>'Leaderboard 1'!A4</f>
+        <f>Leaderboards!A4</f>
         <v>d s</v>
       </c>
       <c r="E5" s="9"/>
@@ -6168,7 +6180,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="26" t="str">
-        <f>'Leaderboard 1'!A5</f>
+        <f>Leaderboards!A5</f>
         <v>w n</v>
       </c>
       <c r="E6" s="9"/>
@@ -6220,7 +6232,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="26" t="str">
-        <f>'Leaderboard 1'!A6</f>
+        <f>Leaderboards!A6</f>
         <v>q w</v>
       </c>
       <c r="E7" s="9"/>
@@ -6272,7 +6284,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="26" t="str">
-        <f>'Leaderboard 1'!A7</f>
+        <f>Leaderboards!A7</f>
         <v>r q</v>
       </c>
       <c r="E8" s="9"/>
@@ -6324,7 +6336,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="26" t="str">
-        <f>'Leaderboard 1'!A8</f>
+        <f>Leaderboards!A8</f>
         <v>r q</v>
       </c>
       <c r="E9" s="9"/>
@@ -6376,7 +6388,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="26" t="str">
-        <f>'Leaderboard 1'!A9</f>
+        <f>Leaderboards!A9</f>
         <v>r q</v>
       </c>
       <c r="E10" s="9"/>
@@ -6428,7 +6440,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="26" t="str">
-        <f>'Leaderboard 1'!A10</f>
+        <f>Leaderboards!A10</f>
         <v>r q</v>
       </c>
       <c r="E11" s="9"/>
@@ -6480,7 +6492,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="26" t="str">
-        <f>'Leaderboard 1'!A11</f>
+        <f>Leaderboards!A11</f>
         <v>r q</v>
       </c>
       <c r="E12" s="9"/>
@@ -6532,7 +6544,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="26" t="str">
-        <f>'Leaderboard 1'!A12</f>
+        <f>Leaderboards!A12</f>
         <v>r q</v>
       </c>
       <c r="E13" s="9"/>
@@ -6584,7 +6596,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="26" t="str">
-        <f>'Leaderboard 1'!A13</f>
+        <f>Leaderboards!A13</f>
         <v>r q</v>
       </c>
       <c r="E14" s="9"/>
@@ -6636,7 +6648,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="26" t="str">
-        <f>'Leaderboard 1'!A14</f>
+        <f>Leaderboards!A14</f>
         <v>r q</v>
       </c>
       <c r="E15" s="9"/>
@@ -6682,7 +6694,7 @@
     </row>
     <row r="16" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D16" s="26" t="str">
-        <f>'Leaderboard 1'!A15</f>
+        <f>Leaderboards!A15</f>
         <v>r q</v>
       </c>
       <c r="E16" s="11"/>
@@ -6855,7 +6867,7 @@
     </row>
     <row r="23" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D23" s="26" t="str">
-        <f>'Leaderboard 1'!A22</f>
+        <f>Leaderboards!A22</f>
         <v>s g</v>
       </c>
       <c r="E23" s="9"/>
@@ -6901,7 +6913,7 @@
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D24" s="26" t="str">
-        <f>'Leaderboard 1'!A23</f>
+        <f>Leaderboards!A23</f>
         <v>a g</v>
       </c>
       <c r="E24" s="9"/>
@@ -6947,7 +6959,7 @@
     </row>
     <row r="25" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D25" s="26" t="str">
-        <f>'Leaderboard 1'!A24</f>
+        <f>Leaderboards!A24</f>
         <v>c dg</v>
       </c>
       <c r="E25" s="9"/>
@@ -6993,7 +7005,7 @@
     </row>
     <row r="26" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D26" s="26" t="str">
-        <f>'Leaderboard 1'!A25</f>
+        <f>Leaderboards!A25</f>
         <v>i d</v>
       </c>
       <c r="E26" s="9"/>
@@ -7039,7 +7051,7 @@
     </row>
     <row r="27" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D27" s="26" t="str">
-        <f>'Leaderboard 1'!A26</f>
+        <f>Leaderboards!A26</f>
         <v>s g</v>
       </c>
       <c r="E27" s="9"/>
@@ -7085,7 +7097,7 @@
     </row>
     <row r="28" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D28" s="26" t="str">
-        <f>'Leaderboard 1'!A27</f>
+        <f>Leaderboards!A27</f>
         <v>a a</v>
       </c>
       <c r="E28" s="9"/>
@@ -7131,7 +7143,7 @@
     </row>
     <row r="29" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D29" s="26" t="str">
-        <f>'Leaderboard 1'!A28</f>
+        <f>Leaderboards!A28</f>
         <v>c sa</v>
       </c>
       <c r="E29" s="9"/>
@@ -7177,7 +7189,7 @@
     </row>
     <row r="30" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D30" s="26" t="str">
-        <f>'Leaderboard 1'!A29</f>
+        <f>Leaderboards!A29</f>
         <v>i d</v>
       </c>
       <c r="E30" s="9"/>
@@ -7223,7 +7235,7 @@
     </row>
     <row r="31" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D31" s="26" t="str">
-        <f>'Leaderboard 1'!A30</f>
+        <f>Leaderboards!A30</f>
         <v>s f</v>
       </c>
       <c r="E31" s="9"/>
@@ -7269,7 +7281,7 @@
     </row>
     <row r="32" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D32" s="26" t="str">
-        <f>'Leaderboard 1'!A31</f>
+        <f>Leaderboards!A31</f>
         <v>a d</v>
       </c>
       <c r="E32" s="9"/>
@@ -7315,7 +7327,7 @@
     </row>
     <row r="33" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D33" s="26" t="str">
-        <f>'Leaderboard 1'!A32</f>
+        <f>Leaderboards!A32</f>
         <v>c a</v>
       </c>
       <c r="E33" s="9"/>
@@ -7361,7 +7373,7 @@
     </row>
     <row r="34" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D34" s="26">
-        <f>'Leaderboard 1'!A33</f>
+        <f>Leaderboards!A33</f>
         <v>0</v>
       </c>
       <c r="E34" s="11"/>
@@ -7534,7 +7546,7 @@
     </row>
     <row r="41" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D41" s="26" t="str">
-        <f>'Leaderboard 1'!M4</f>
+        <f>Leaderboards!M4</f>
         <v>g j</v>
       </c>
       <c r="E41" s="9"/>
@@ -7580,7 +7592,7 @@
     </row>
     <row r="42" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D42" s="26" t="str">
-        <f>'Leaderboard 1'!M5</f>
+        <f>Leaderboards!M5</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E42" s="9"/>
@@ -7626,7 +7638,7 @@
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D43" s="26" t="str">
-        <f>'Leaderboard 1'!M6</f>
+        <f>Leaderboards!M6</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E43" s="9"/>
@@ -7672,7 +7684,7 @@
     </row>
     <row r="44" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D44" s="26" t="str">
-        <f>'Leaderboard 1'!M7</f>
+        <f>Leaderboards!M7</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E44" s="9"/>
@@ -7718,7 +7730,7 @@
     </row>
     <row r="45" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D45" s="26" t="str">
-        <f>'Leaderboard 1'!M8</f>
+        <f>Leaderboards!M8</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E45" s="9"/>
@@ -7764,7 +7776,7 @@
     </row>
     <row r="46" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D46" s="26" t="str">
-        <f>'Leaderboard 1'!M9</f>
+        <f>Leaderboards!M9</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E46" s="9"/>
@@ -7810,7 +7822,7 @@
     </row>
     <row r="47" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D47" s="26" t="str">
-        <f>'Leaderboard 1'!M10</f>
+        <f>Leaderboards!M10</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E47" s="9"/>
@@ -7856,7 +7868,7 @@
     </row>
     <row r="48" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D48" s="26" t="str">
-        <f>'Leaderboard 1'!M11</f>
+        <f>Leaderboards!M11</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E48" s="9"/>
@@ -7902,7 +7914,7 @@
     </row>
     <row r="49" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D49" s="26" t="str">
-        <f>'Leaderboard 1'!M12</f>
+        <f>Leaderboards!M12</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E49" s="9"/>
@@ -7948,7 +7960,7 @@
     </row>
     <row r="50" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D50" s="26" t="str">
-        <f>'Leaderboard 1'!M13</f>
+        <f>Leaderboards!M13</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E50" s="9"/>
@@ -7994,7 +8006,7 @@
     </row>
     <row r="51" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D51" s="26" t="str">
-        <f>'Leaderboard 1'!M14</f>
+        <f>Leaderboards!M14</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E51" s="9"/>
@@ -8040,7 +8052,7 @@
     </row>
     <row r="52" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D52" s="26" t="str">
-        <f>'Leaderboard 1'!M15</f>
+        <f>Leaderboards!M15</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E52" s="11"/>
@@ -8213,7 +8225,7 @@
     </row>
     <row r="59" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D59" s="26" t="str">
-        <f>'Leaderboard 1'!M21</f>
+        <f>Leaderboards!M21</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E59" s="9"/>
@@ -8259,7 +8271,7 @@
     </row>
     <row r="60" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D60" s="26" t="str">
-        <f>'Leaderboard 1'!M22</f>
+        <f>Leaderboards!M22</f>
         <v>g f</v>
       </c>
       <c r="E60" s="9"/>
@@ -8305,7 +8317,7 @@
     </row>
     <row r="61" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D61" s="26" t="str">
-        <f>'Leaderboard 1'!M23</f>
+        <f>Leaderboards!M23</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E61" s="9"/>
@@ -8351,7 +8363,7 @@
     </row>
     <row r="62" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D62" s="26" t="str">
-        <f>'Leaderboard 1'!M24</f>
+        <f>Leaderboards!M24</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E62" s="9"/>
@@ -8397,7 +8409,7 @@
     </row>
     <row r="63" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D63" s="26" t="str">
-        <f>'Leaderboard 1'!M25</f>
+        <f>Leaderboards!M25</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E63" s="9"/>
@@ -8443,7 +8455,7 @@
     </row>
     <row r="64" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D64" s="26" t="str">
-        <f>'Leaderboard 1'!M26</f>
+        <f>Leaderboards!M26</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E64" s="9"/>
@@ -8489,7 +8501,7 @@
     </row>
     <row r="65" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D65" s="26" t="str">
-        <f>'Leaderboard 1'!M27</f>
+        <f>Leaderboards!M27</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E65" s="9"/>
@@ -8535,7 +8547,7 @@
     </row>
     <row r="66" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D66" s="26" t="str">
-        <f>'Leaderboard 1'!M28</f>
+        <f>Leaderboards!M28</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E66" s="9"/>
@@ -8581,7 +8593,7 @@
     </row>
     <row r="67" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D67" s="26" t="str">
-        <f>'Leaderboard 1'!M29</f>
+        <f>Leaderboards!M29</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E67" s="9"/>
@@ -8627,7 +8639,7 @@
     </row>
     <row r="68" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D68" s="26" t="str">
-        <f>'Leaderboard 1'!M30</f>
+        <f>Leaderboards!M30</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E68" s="9"/>
@@ -8673,7 +8685,7 @@
     </row>
     <row r="69" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D69" s="26" t="str">
-        <f>'Leaderboard 1'!M31</f>
+        <f>Leaderboards!M31</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E69" s="9"/>
@@ -8719,7 +8731,7 @@
     </row>
     <row r="70" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D70" s="26" t="str">
-        <f>'Leaderboard 1'!M32</f>
+        <f>Leaderboards!M32</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E70" s="11"/>

</xml_diff>

<commit_message>
i dont even remember the changes
</commit_message>
<xml_diff>
--- a/league template.xlsx
+++ b/league template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goftaps-my.sharepoint.com/personal/sstaley_gofullthrottle_com/Documents/excel stuff/leagues/League-Points-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="655" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2945338F-C519-4FB1-8B63-58A8A1DCC642}"/>
+  <xr:revisionPtr revIDLastSave="673" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD309661-8B5B-4DC3-9EF7-76A74297B6C7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -125,52 +125,7 @@
     <t>*Only edit points in the points calculator sheet*</t>
   </si>
   <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>dg</t>
   </si>
   <si>
     <t>Kart times pulled from: 8/12 - 8/19</t>
@@ -3221,7 +3176,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3307,30 +3262,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C4" s="13">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="13">
         <v>40</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="K4" s="13">
         <v>40</v>
       </c>
@@ -3339,53 +3276,23 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C5" s="13">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G5" s="13">
         <v>0</v>
       </c>
       <c r="K5" s="13">
         <v>0</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O5" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C6" s="13">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G6" s="13">
         <v>0</v>
       </c>
@@ -3397,21 +3304,9 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="13">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="13">
         <v>0</v>
       </c>
@@ -3423,21 +3318,9 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C8" s="13">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G8" s="13">
         <v>0</v>
       </c>
@@ -3449,21 +3332,9 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C9" s="13">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G9" s="13">
         <v>0</v>
       </c>
@@ -3475,21 +3346,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C10" s="13">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G10" s="13">
         <v>0</v>
       </c>
@@ -3501,21 +3360,9 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C11" s="13">
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="G11" s="13">
         <v>0</v>
       </c>
@@ -3527,21 +3374,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C12" s="13">
         <v>0</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G12" s="13">
         <v>0</v>
       </c>
@@ -3553,21 +3388,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C13" s="13">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="G13" s="13">
         <v>0</v>
       </c>
@@ -3579,21 +3402,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="13">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G14" s="13">
         <v>0</v>
       </c>
@@ -3605,20 +3416,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="13">
         <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="G15" s="13">
         <v>0</v>
@@ -3692,7 +3491,7 @@
   </sheetPr>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:J19"/>
     </sheetView>
   </sheetViews>
@@ -3814,7 +3613,7 @@
     <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>CONCATENATE(Roster!A4, " ", Roster!B4)</f>
-        <v>d s</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B4">
         <f>'Points calculator'!F5</f>
@@ -3849,12 +3648,12 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f>SUM(B4:I4) - MIN(B4:I4)</f>
+        <f t="shared" ref="J4:J15" si="0">SUM(B4:I4) - MIN(B4:I4)</f>
         <v>0</v>
       </c>
       <c r="M4" t="str">
         <f>CONCATENATE(roster_division3[[#This Row],[First Name]], " ", roster_division3[[#This Row],[Last Name]])</f>
-        <v>g j</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="N4">
         <f>'Points calculator'!F41</f>
@@ -3889,14 +3688,14 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <f>SUM(N4:U4) - MIN(N4:U4)</f>
+        <f t="shared" ref="V4:V15" si="1">SUM(N4:U4) - MIN(N4:U4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>CONCATENATE(Roster!A5, " ", Roster!B5)</f>
-        <v>w n</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B5">
         <f>'Points calculator'!F6</f>
@@ -3931,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <f>SUM(B5:I5) - MIN(B5:I5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M5" t="str">
@@ -3971,14 +3770,14 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <f>SUM(N5:U5) - MIN(N5:U5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f>CONCATENATE(Roster!A6, " ", Roster!B6)</f>
-        <v>q w</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B6">
         <f>'Points calculator'!F7</f>
@@ -4013,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <f>SUM(B6:I6) - MIN(B6:I6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M6" t="str">
@@ -4053,14 +3852,14 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <f>SUM(N6:U6) - MIN(N6:U6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>CONCATENATE(Roster!A7, " ", Roster!B7)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B7">
         <f>'Points calculator'!F8</f>
@@ -4095,7 +3894,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <f>SUM(B7:I7) - MIN(B7:I7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M7" t="str">
@@ -4135,14 +3934,14 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <f>SUM(N7:U7) - MIN(N7:U7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>CONCATENATE(Roster!A8, " ", Roster!B8)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B8">
         <f>'Points calculator'!F9</f>
@@ -4177,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <f>SUM(B8:I8) - MIN(B8:I8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M8" t="str">
@@ -4217,14 +4016,14 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <f>SUM(N8:U8) - MIN(N8:U8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f>CONCATENATE(Roster!A9, " ", Roster!B9)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B9">
         <f>'Points calculator'!F10</f>
@@ -4259,7 +4058,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <f>SUM(B9:I9) - MIN(B9:I9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M9" t="str">
@@ -4299,14 +4098,14 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <f>SUM(N9:U9) - MIN(N9:U9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>CONCATENATE(Roster!A10, " ", Roster!B10)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B10">
         <f>'Points calculator'!F11</f>
@@ -4341,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <f>SUM(B10:I10) - MIN(B10:I10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M10" t="str">
@@ -4381,14 +4180,14 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <f>SUM(N10:U10) - MIN(N10:U10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f>CONCATENATE(Roster!A11, " ", Roster!B11)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B11">
         <f>'Points calculator'!F12</f>
@@ -4423,7 +4222,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <f>SUM(B11:I11) - MIN(B11:I11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M11" t="str">
@@ -4463,14 +4262,14 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <f>SUM(N11:U11) - MIN(N11:U11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f>CONCATENATE(Roster!A12, " ", Roster!B12)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B12">
         <f>'Points calculator'!F13</f>
@@ -4505,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <f>SUM(B12:I12) - MIN(B12:I12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12" t="str">
@@ -4545,14 +4344,14 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <f>SUM(N12:U12) - MIN(N12:U12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f>CONCATENATE(Roster!A13, " ", Roster!B13)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B13">
         <f>'Points calculator'!F14</f>
@@ -4587,7 +4386,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <f>SUM(B13:I13) - MIN(B13:I13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M13" t="str">
@@ -4627,14 +4426,14 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <f>SUM(N13:U13) - MIN(N13:U13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>CONCATENATE(Roster!A14, " ", Roster!B14)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B14">
         <f>'Points calculator'!F15</f>
@@ -4669,7 +4468,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <f>SUM(B14:I14) - MIN(B14:I14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M14" t="str">
@@ -4709,14 +4508,14 @@
         <v>0</v>
       </c>
       <c r="V14">
-        <f>SUM(N14:U14) - MIN(N14:U14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>CONCATENATE(Roster!A15, " ", Roster!B15)</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B15">
         <f>'Points calculator'!F16</f>
@@ -4751,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <f>SUM(B15:I15) - MIN(B15:I15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15" t="str">
@@ -4791,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="V15">
-        <f>SUM(N15:U15) - MIN(N15:U15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4924,7 +4723,7 @@
     <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
         <f>CONCATENATE(Roster!E4, " ", Roster!F4)</f>
-        <v>i u</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B21">
         <f>'Points calculator'!F23</f>
@@ -4959,7 +4758,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <f>SUM(B21:I21) - MIN(B21:I21)</f>
+        <f t="shared" ref="J21:J32" si="2">SUM(B21:I21) - MIN(B21:I21)</f>
         <v>0</v>
       </c>
       <c r="M21" t="str">
@@ -4999,14 +4798,14 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <f>SUM(N21:U21) - MIN(N21:U21)</f>
+        <f t="shared" ref="V21:V32" si="3">SUM(N21:U21) - MIN(N21:U21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" t="str">
         <f>CONCATENATE(Roster!E5, " ", Roster!F5)</f>
-        <v>s g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B22">
         <f>'Points calculator'!F24</f>
@@ -5041,12 +4840,12 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f>SUM(B22:I22) - MIN(B22:I22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M22" t="str">
         <f>CONCATENATE(Roster!M5, " ", Roster!N5)</f>
-        <v>g f</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="N22">
         <f>'Points calculator'!F60</f>
@@ -5081,14 +4880,14 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <f>SUM(N22:U22) - MIN(N22:U22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
         <f>CONCATENATE(Roster!E6, " ", Roster!F6)</f>
-        <v>a g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B23">
         <f>'Points calculator'!F25</f>
@@ -5123,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f>SUM(B23:I23) - MIN(B23:I23)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23" t="str">
@@ -5163,14 +4962,14 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <f>SUM(N23:U23) - MIN(N23:U23)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" t="str">
         <f>CONCATENATE(Roster!E7, " ", Roster!F7)</f>
-        <v>c dg</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B24">
         <f>'Points calculator'!F26</f>
@@ -5205,7 +5004,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f>SUM(B24:I24) - MIN(B24:I24)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24" t="str">
@@ -5245,14 +5044,14 @@
         <v>0</v>
       </c>
       <c r="V24">
-        <f>SUM(N24:U24) - MIN(N24:U24)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25" t="str">
         <f>CONCATENATE(Roster!E8, " ", Roster!F8)</f>
-        <v>i d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B25">
         <f>'Points calculator'!F27</f>
@@ -5287,7 +5086,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <f>SUM(B25:I25) - MIN(B25:I25)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M25" t="str">
@@ -5327,14 +5126,14 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <f>SUM(N25:U25) - MIN(N25:U25)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f>CONCATENATE(Roster!E9, " ", Roster!F9)</f>
-        <v>s g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B26">
         <f>'Points calculator'!F28</f>
@@ -5369,7 +5168,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <f>SUM(B26:I26) - MIN(B26:I26)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M26" t="str">
@@ -5409,14 +5208,14 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <f>SUM(N26:U26) - MIN(N26:U26)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f>CONCATENATE(Roster!E10, " ", Roster!F10)</f>
-        <v>a a</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B27">
         <f>'Points calculator'!F29</f>
@@ -5451,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <f>SUM(B27:I27) - MIN(B27:I27)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M27" t="str">
@@ -5491,14 +5290,14 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <f>SUM(N27:U27) - MIN(N27:U27)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f>CONCATENATE(Roster!E11, " ", Roster!F11)</f>
-        <v>c sa</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B28">
         <f>'Points calculator'!F30</f>
@@ -5533,7 +5332,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <f>SUM(B28:I28) - MIN(B28:I28)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M28" t="str">
@@ -5573,14 +5372,14 @@
         <v>0</v>
       </c>
       <c r="V28">
-        <f>SUM(N28:U28) - MIN(N28:U28)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <f>CONCATENATE(Roster!E12, " ", Roster!F12)</f>
-        <v>i d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B29">
         <f>'Points calculator'!F31</f>
@@ -5615,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <f>SUM(B29:I29) - MIN(B29:I29)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M29" t="str">
@@ -5655,14 +5454,14 @@
         <v>0</v>
       </c>
       <c r="V29">
-        <f>SUM(N29:U29) - MIN(N29:U29)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
         <f>CONCATENATE(Roster!E13, " ", Roster!F13)</f>
-        <v>s f</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B30">
         <f>'Points calculator'!F32</f>
@@ -5697,7 +5496,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <f>SUM(B30:I30) - MIN(B30:I30)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M30" t="str">
@@ -5737,14 +5536,14 @@
         <v>0</v>
       </c>
       <c r="V30">
-        <f>SUM(N30:U30) - MIN(N30:U30)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
         <f>CONCATENATE(Roster!E14, " ", Roster!F14)</f>
-        <v>a d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B31">
         <f>'Points calculator'!F33</f>
@@ -5779,7 +5578,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <f>SUM(B31:I31) - MIN(B31:I31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M31" t="str">
@@ -5819,14 +5618,14 @@
         <v>0</v>
       </c>
       <c r="V31">
-        <f>SUM(N31:U31) - MIN(N31:U31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32" t="str">
         <f>CONCATENATE(Roster!E15, " ", Roster!F15)</f>
-        <v>c a</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B32">
         <f>'Points calculator'!F34</f>
@@ -5861,7 +5660,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <f>SUM(B32:I32) - MIN(B32:I32)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M32" t="str">
@@ -5901,7 +5700,7 @@
         <v>0</v>
       </c>
       <c r="V32">
-        <f>SUM(N32:U32) - MIN(N32:U32)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5944,8 +5743,8 @@
   </sheetPr>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView topLeftCell="C45" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6129,7 +5928,7 @@
       </c>
       <c r="D5" s="26" t="str">
         <f>Leaderboards!A4</f>
-        <v>d s</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="27">
@@ -6181,7 +5980,7 @@
       </c>
       <c r="D6" s="26" t="str">
         <f>Leaderboards!A5</f>
-        <v>w n</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="27">
@@ -6233,7 +6032,7 @@
       </c>
       <c r="D7" s="26" t="str">
         <f>Leaderboards!A6</f>
-        <v>q w</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="27">
@@ -6285,7 +6084,7 @@
       </c>
       <c r="D8" s="26" t="str">
         <f>Leaderboards!A7</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="27">
@@ -6337,7 +6136,7 @@
       </c>
       <c r="D9" s="26" t="str">
         <f>Leaderboards!A8</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="27">
@@ -6389,7 +6188,7 @@
       </c>
       <c r="D10" s="26" t="str">
         <f>Leaderboards!A9</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="27">
@@ -6441,7 +6240,7 @@
       </c>
       <c r="D11" s="26" t="str">
         <f>Leaderboards!A10</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="27">
@@ -6493,7 +6292,7 @@
       </c>
       <c r="D12" s="26" t="str">
         <f>Leaderboards!A11</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="27">
@@ -6545,7 +6344,7 @@
       </c>
       <c r="D13" s="26" t="str">
         <f>Leaderboards!A12</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="27">
@@ -6597,7 +6396,7 @@
       </c>
       <c r="D14" s="26" t="str">
         <f>Leaderboards!A13</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="27">
@@ -6649,7 +6448,7 @@
       </c>
       <c r="D15" s="26" t="str">
         <f>Leaderboards!A14</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="27">
@@ -6695,7 +6494,7 @@
     <row r="16" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D16" s="26" t="str">
         <f>Leaderboards!A15</f>
-        <v>r q</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="27">
@@ -6868,7 +6667,7 @@
     <row r="23" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D23" s="26" t="str">
         <f>Leaderboards!A22</f>
-        <v>s g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="27">
@@ -6914,7 +6713,7 @@
     <row r="24" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D24" s="26" t="str">
         <f>Leaderboards!A23</f>
-        <v>a g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="27">
@@ -6960,7 +6759,7 @@
     <row r="25" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D25" s="26" t="str">
         <f>Leaderboards!A24</f>
-        <v>c dg</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="27">
@@ -7006,7 +6805,7 @@
     <row r="26" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D26" s="26" t="str">
         <f>Leaderboards!A25</f>
-        <v>i d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="27">
@@ -7052,7 +6851,7 @@
     <row r="27" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D27" s="26" t="str">
         <f>Leaderboards!A26</f>
-        <v>s g</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="27">
@@ -7098,7 +6897,7 @@
     <row r="28" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D28" s="26" t="str">
         <f>Leaderboards!A27</f>
-        <v>a a</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="27">
@@ -7144,7 +6943,7 @@
     <row r="29" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D29" s="26" t="str">
         <f>Leaderboards!A28</f>
-        <v>c sa</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="27">
@@ -7190,7 +6989,7 @@
     <row r="30" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D30" s="26" t="str">
         <f>Leaderboards!A29</f>
-        <v>i d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="27">
@@ -7236,7 +7035,7 @@
     <row r="31" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D31" s="26" t="str">
         <f>Leaderboards!A30</f>
-        <v>s f</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="27">
@@ -7282,7 +7081,7 @@
     <row r="32" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D32" s="26" t="str">
         <f>Leaderboards!A31</f>
-        <v>a d</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="27">
@@ -7328,7 +7127,7 @@
     <row r="33" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D33" s="26" t="str">
         <f>Leaderboards!A32</f>
-        <v>c a</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="27">
@@ -7547,7 +7346,7 @@
     <row r="41" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D41" s="26" t="str">
         <f>Leaderboards!M4</f>
-        <v>g j</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="27">
@@ -8272,7 +8071,7 @@
     <row r="60" spans="4:20" x14ac:dyDescent="0.45">
       <c r="D60" s="26" t="str">
         <f>Leaderboards!M22</f>
-        <v>g f</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="27">
@@ -8854,7 +8653,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -8867,9 +8666,9 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="I2" t="str">
+      <c r="I2">
         <f>Roster!I4</f>
-        <v>g</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
         <f>Roster!K4</f>
@@ -9047,7 +8846,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="38" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
@@ -9141,7 +8940,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -9152,9 +8951,9 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
-      <c r="I2" t="str">
+      <c r="I2">
         <f>Roster!A4</f>
-        <v>d</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
         <f>Roster!C4</f>
@@ -9163,9 +8962,9 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
-      <c r="I3" t="str">
+      <c r="I3">
         <f>Roster!A5</f>
-        <v>w</v>
+        <v>0</v>
       </c>
       <c r="J3" s="14">
         <f>Roster!C5</f>
@@ -9174,9 +8973,9 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
-      <c r="I4" t="str">
+      <c r="I4">
         <f>Roster!A6</f>
-        <v>q</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
         <f>Roster!C6</f>
@@ -9185,9 +8984,9 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
-      <c r="I5" t="str">
+      <c r="I5">
         <f>Roster!A7</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J5" s="14">
         <f>Roster!C7</f>
@@ -9196,9 +8995,9 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
-      <c r="I6" t="str">
+      <c r="I6">
         <f>Roster!A8</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J6" s="14">
         <f>Roster!C8</f>
@@ -9207,9 +9006,9 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="I7" t="str">
+      <c r="I7">
         <f>Roster!A9</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J7" s="14">
         <f>Roster!C9</f>
@@ -9218,9 +9017,9 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="I8" t="str">
+      <c r="I8">
         <f>Roster!A10</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J8" s="14">
         <f>Roster!C10</f>
@@ -9229,9 +9028,9 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
-      <c r="I9" t="str">
+      <c r="I9">
         <f>Roster!A11</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J9" s="14">
         <f>Roster!C11</f>
@@ -9240,9 +9039,9 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
-      <c r="I10" t="str">
+      <c r="I10">
         <f>Roster!A12</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J10" s="14">
         <f>Roster!C12</f>
@@ -9251,9 +9050,9 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
-      <c r="I11" t="str">
+      <c r="I11">
         <f>Roster!A13</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J11" s="14">
         <f>Roster!C13</f>
@@ -9262,9 +9061,9 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
-      <c r="I12" t="str">
+      <c r="I12">
         <f>Roster!A14</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J12" s="14">
         <f>Roster!C14</f>
@@ -9273,9 +9072,9 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
-      <c r="I13" t="str">
+      <c r="I13">
         <f>Roster!A15</f>
-        <v>r</v>
+        <v>0</v>
       </c>
       <c r="J13" s="14">
         <f>Roster!C15</f>
@@ -9402,7 +9201,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -9424,9 +9223,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2" t="str">
+      <c r="I2">
         <f>Roster!E4</f>
-        <v>i</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
         <f>Roster!G4</f>
@@ -9446,9 +9245,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3">
         <f>Roster!E5</f>
-        <v>s</v>
+        <v>0</v>
       </c>
       <c r="J3" s="14">
         <f>Roster!G5</f>
@@ -9468,9 +9267,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I4">
         <f>Roster!E6</f>
-        <v>a</v>
+        <v>0</v>
       </c>
       <c r="J4" s="14">
         <f>Roster!G6</f>
@@ -9490,9 +9289,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I5" t="str">
+      <c r="I5">
         <f>Roster!E7</f>
-        <v>c</v>
+        <v>0</v>
       </c>
       <c r="J5" s="14">
         <f>Roster!G7</f>
@@ -9512,9 +9311,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I6">
         <f>Roster!E8</f>
-        <v>i</v>
+        <v>0</v>
       </c>
       <c r="J6" s="14">
         <f>Roster!G8</f>
@@ -9534,9 +9333,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I7">
         <f>Roster!E9</f>
-        <v>s</v>
+        <v>0</v>
       </c>
       <c r="J7" s="14">
         <f>Roster!G9</f>
@@ -9556,9 +9355,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I8" t="str">
+      <c r="I8">
         <f>Roster!E10</f>
-        <v>a</v>
+        <v>0</v>
       </c>
       <c r="J8" s="14">
         <f>Roster!G10</f>
@@ -9578,9 +9377,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I9" t="str">
+      <c r="I9">
         <f>Roster!E11</f>
-        <v>c</v>
+        <v>0</v>
       </c>
       <c r="J9" s="14">
         <f>Roster!G11</f>
@@ -9600,9 +9399,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I10" t="str">
+      <c r="I10">
         <f>Roster!E12</f>
-        <v>i</v>
+        <v>0</v>
       </c>
       <c r="J10" s="14">
         <f>Roster!G12</f>
@@ -9622,9 +9421,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I11" t="str">
+      <c r="I11">
         <f>Roster!E13</f>
-        <v>s</v>
+        <v>0</v>
       </c>
       <c r="J11" s="14">
         <f>Roster!G13</f>
@@ -9644,9 +9443,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I12" t="str">
+      <c r="I12">
         <f>Roster!E14</f>
-        <v>a</v>
+        <v>0</v>
       </c>
       <c r="J12" s="14">
         <f>Roster!G14</f>
@@ -9666,9 +9465,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I13" t="str">
+      <c r="I13">
         <f>Roster!E15</f>
-        <v>c</v>
+        <v>0</v>
       </c>
       <c r="J13" s="14">
         <f>Roster!G15</f>
@@ -9818,7 +9617,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -9840,9 +9639,9 @@
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2" t="str">
+      <c r="I2">
         <f>Roster!I4</f>
-        <v>g</v>
+        <v>0</v>
       </c>
       <c r="J2" s="14">
         <f>Roster!K4</f>

</xml_diff>

<commit_message>
updated protections on excel sheet
</commit_message>
<xml_diff>
--- a/league template.xlsx
+++ b/league template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goftaps-my.sharepoint.com/personal/sstaley_gofullthrottle_com/Documents/excel stuff/leagues/League-Points-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="673" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD309661-8B5B-4DC3-9EF7-76A74297B6C7}"/>
+  <xr:revisionPtr revIDLastSave="703" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DDA672C-BBCB-41D5-A2FE-EE3D9CDB14BE}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="3" r:id="rId1"/>
@@ -128,7 +128,7 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Kart times pulled from: 8/12 - 8/19</t>
+    <t>Kart times pulled from: 8/18 - 8/25</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -562,11 +562,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="261">
+  <dxfs count="263">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -608,114 +721,15 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -2441,142 +2455,142 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8A66A64-948E-45A2-8B35-E39203DBCA86}" name="roster_division1" displayName="roster_division1" ref="A3:C15" totalsRowShown="0" headerRowDxfId="260" dataDxfId="259">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8A66A64-948E-45A2-8B35-E39203DBCA86}" name="roster_division1" displayName="roster_division1" ref="A3:C15" totalsRowShown="0" headerRowDxfId="262" dataDxfId="261">
   <autoFilter ref="A3:C15" xr:uid="{E8A66A64-948E-45A2-8B35-E39203DBCA86}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1B6D1E9E-3474-4EAF-95CE-7635638EB2D7}" name="First Name" dataDxfId="258"/>
-    <tableColumn id="2" xr3:uid="{A331963E-6AAC-4617-A399-8E5083B7A1FE}" name="Last Name" dataDxfId="257"/>
-    <tableColumn id="3" xr3:uid="{D9653975-D6FF-407F-99AF-04C3CCF11B66}" name="Weight" dataDxfId="256"/>
+    <tableColumn id="1" xr3:uid="{1B6D1E9E-3474-4EAF-95CE-7635638EB2D7}" name="First Name" dataDxfId="260"/>
+    <tableColumn id="2" xr3:uid="{A331963E-6AAC-4617-A399-8E5083B7A1FE}" name="Last Name" dataDxfId="259"/>
+    <tableColumn id="3" xr3:uid="{D9653975-D6FF-407F-99AF-04C3CCF11B66}" name="Weight" dataDxfId="258"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{413CA066-BE2B-49DE-9452-0AE4E5D4A4CE}" name="pointscalculator_division1" displayName="pointscalculator_division1" ref="D3:T16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{413CA066-BE2B-49DE-9452-0AE4E5D4A4CE}" name="pointscalculator_division1" displayName="pointscalculator_division1" ref="D3:T16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="187" dataDxfId="186">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{F54777DC-034B-4405-846B-D85CB4398F34}" name="Column1" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{87828A0C-FB90-4EA4-9B26-E5EA357BACC8}" name="Column2" headerRowDxfId="182" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{7933F018-C288-4807-985F-73CE9EFB4BBF}" name="Column3" headerRowDxfId="180" dataDxfId="179"/>
-    <tableColumn id="4" xr3:uid="{CEE14F89-D085-484E-B88A-6785163384C7}" name="Column4" headerRowDxfId="178" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{EDD514C2-D109-4B2F-9958-5D6E893B230D}" name="Column5" headerRowDxfId="176" dataDxfId="175"/>
-    <tableColumn id="6" xr3:uid="{11AC3DAF-2D1D-413C-A77A-2000CFA42613}" name="Column6" headerRowDxfId="174" dataDxfId="173"/>
-    <tableColumn id="7" xr3:uid="{1A6E6C30-0A25-43CE-8344-4A67CA14F6B6}" name="Column7" headerRowDxfId="172" dataDxfId="171"/>
-    <tableColumn id="8" xr3:uid="{71045566-6F44-4D03-ACB4-1F9B882EF703}" name="Column8" headerRowDxfId="170" dataDxfId="169"/>
-    <tableColumn id="9" xr3:uid="{EFA47D07-D6E3-437E-8FA1-A833AAF189FD}" name="Column9" headerRowDxfId="168" dataDxfId="167"/>
-    <tableColumn id="10" xr3:uid="{94A4BF73-A2A3-4928-AC13-700E2832FD15}" name="Column10" headerRowDxfId="166" dataDxfId="165"/>
-    <tableColumn id="11" xr3:uid="{9D7E6C6D-E940-4FBF-9363-95A8A6BB59CB}" name="Column11" headerRowDxfId="164" dataDxfId="163"/>
-    <tableColumn id="12" xr3:uid="{E85E09B6-3A31-4149-9FF1-4AB41A9C2E92}" name="Column12" headerRowDxfId="162" dataDxfId="161"/>
-    <tableColumn id="13" xr3:uid="{BC746882-1E84-4472-9C57-BD0D76DB39C8}" name="Column13" headerRowDxfId="160" dataDxfId="159"/>
-    <tableColumn id="14" xr3:uid="{6139B53E-4C13-45B2-8A9B-7F61D0A66175}" name="Column14" headerRowDxfId="158" dataDxfId="157"/>
-    <tableColumn id="15" xr3:uid="{E7FBC0E6-A070-48A4-9E06-7041DEC79D91}" name="Column15" headerRowDxfId="156" dataDxfId="155"/>
-    <tableColumn id="16" xr3:uid="{821CC151-5CEF-492B-824A-D2BED3D1DFEB}" name="Column16" headerRowDxfId="154" dataDxfId="153"/>
-    <tableColumn id="17" xr3:uid="{41E5B94B-F427-49FB-9779-C3AF379CFA71}" name="Column17" headerRowDxfId="152" dataDxfId="151"/>
+    <tableColumn id="1" xr3:uid="{F54777DC-034B-4405-846B-D85CB4398F34}" name="Column1" dataDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{87828A0C-FB90-4EA4-9B26-E5EA357BACC8}" name="Column2" headerRowDxfId="184" dataDxfId="183"/>
+    <tableColumn id="3" xr3:uid="{7933F018-C288-4807-985F-73CE9EFB4BBF}" name="Column3" headerRowDxfId="182" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{CEE14F89-D085-484E-B88A-6785163384C7}" name="Column4" headerRowDxfId="180" dataDxfId="179"/>
+    <tableColumn id="5" xr3:uid="{EDD514C2-D109-4B2F-9958-5D6E893B230D}" name="Column5" headerRowDxfId="178" dataDxfId="177"/>
+    <tableColumn id="6" xr3:uid="{11AC3DAF-2D1D-413C-A77A-2000CFA42613}" name="Column6" headerRowDxfId="176" dataDxfId="175"/>
+    <tableColumn id="7" xr3:uid="{1A6E6C30-0A25-43CE-8344-4A67CA14F6B6}" name="Column7" headerRowDxfId="174" dataDxfId="173"/>
+    <tableColumn id="8" xr3:uid="{71045566-6F44-4D03-ACB4-1F9B882EF703}" name="Column8" headerRowDxfId="172" dataDxfId="171"/>
+    <tableColumn id="9" xr3:uid="{EFA47D07-D6E3-437E-8FA1-A833AAF189FD}" name="Column9" headerRowDxfId="170" dataDxfId="169"/>
+    <tableColumn id="10" xr3:uid="{94A4BF73-A2A3-4928-AC13-700E2832FD15}" name="Column10" headerRowDxfId="168" dataDxfId="167"/>
+    <tableColumn id="11" xr3:uid="{9D7E6C6D-E940-4FBF-9363-95A8A6BB59CB}" name="Column11" headerRowDxfId="166" dataDxfId="165"/>
+    <tableColumn id="12" xr3:uid="{E85E09B6-3A31-4149-9FF1-4AB41A9C2E92}" name="Column12" headerRowDxfId="164" dataDxfId="163"/>
+    <tableColumn id="13" xr3:uid="{BC746882-1E84-4472-9C57-BD0D76DB39C8}" name="Column13" headerRowDxfId="162" dataDxfId="161"/>
+    <tableColumn id="14" xr3:uid="{6139B53E-4C13-45B2-8A9B-7F61D0A66175}" name="Column14" headerRowDxfId="160" dataDxfId="159"/>
+    <tableColumn id="15" xr3:uid="{E7FBC0E6-A070-48A4-9E06-7041DEC79D91}" name="Column15" headerRowDxfId="158" dataDxfId="157"/>
+    <tableColumn id="16" xr3:uid="{821CC151-5CEF-492B-824A-D2BED3D1DFEB}" name="Column16" headerRowDxfId="156" dataDxfId="155"/>
+    <tableColumn id="17" xr3:uid="{41E5B94B-F427-49FB-9779-C3AF379CFA71}" name="Column17" headerRowDxfId="154" dataDxfId="153"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{CBE52FE5-F969-414E-8061-65928C310517}" name="pointscalculator_division2" displayName="pointscalculator_division2" ref="D21:T34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="150" dataDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{CBE52FE5-F969-414E-8061-65928C310517}" name="pointscalculator_division2" displayName="pointscalculator_division2" ref="D21:T34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{A5B7E7CC-F2E9-4C49-BED9-3A47CAE54B7E}" name="Column1" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{1F4A7765-A904-4DF6-B648-094B6BC94FBE}" name="Column2" headerRowDxfId="147" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{839ADCF5-8C6D-4A0C-AAB2-969A42AE8027}" name="Column3" headerRowDxfId="145" dataDxfId="144"/>
-    <tableColumn id="4" xr3:uid="{1731EB37-AE35-486E-855D-77128F4DDF09}" name="Column4" headerRowDxfId="143" dataDxfId="142"/>
-    <tableColumn id="5" xr3:uid="{4F3895B0-C799-4B3D-8759-283BB22EA08E}" name="Column5" headerRowDxfId="141" dataDxfId="140"/>
-    <tableColumn id="6" xr3:uid="{31207C71-AA84-443E-824A-E507F7192E3F}" name="Column6" headerRowDxfId="139" dataDxfId="138"/>
-    <tableColumn id="7" xr3:uid="{3D4AA28B-3E08-4F46-B50A-0C65CF425433}" name="Column7" headerRowDxfId="137" dataDxfId="136"/>
-    <tableColumn id="8" xr3:uid="{64223BBE-3219-453E-AD2C-61C0B9A09904}" name="Column8" headerRowDxfId="135" dataDxfId="134"/>
-    <tableColumn id="9" xr3:uid="{11687BFD-11FB-41C8-B4D4-CDB9E0136019}" name="Column9" headerRowDxfId="133" dataDxfId="132"/>
-    <tableColumn id="10" xr3:uid="{7EF49BEB-C450-4CDD-A592-0945074DF1B6}" name="Column10" headerRowDxfId="131" dataDxfId="130"/>
-    <tableColumn id="11" xr3:uid="{AAA731DE-3024-44C5-83DB-F983987C19BD}" name="Column11" headerRowDxfId="129" dataDxfId="128"/>
-    <tableColumn id="12" xr3:uid="{C2E61F83-831E-4409-9DD2-49A133F6632F}" name="Column12" headerRowDxfId="127" dataDxfId="126"/>
-    <tableColumn id="13" xr3:uid="{36F29327-806B-4BFE-98EF-D858E1BE52B2}" name="Column13" headerRowDxfId="125" dataDxfId="124"/>
-    <tableColumn id="14" xr3:uid="{BAE00B6F-FE30-4E85-AD72-BA5846AF950C}" name="Column14" headerRowDxfId="123" dataDxfId="122"/>
-    <tableColumn id="15" xr3:uid="{56476BC5-A36D-4837-8C13-38FEA912BAC5}" name="Column15" headerRowDxfId="121" dataDxfId="120"/>
-    <tableColumn id="16" xr3:uid="{1C4EAA2A-CB75-4A15-87A1-9CDC9F820B8C}" name="Column16" headerRowDxfId="119" dataDxfId="118"/>
-    <tableColumn id="17" xr3:uid="{C9171481-5E79-493E-A3D8-98929F6931FC}" name="Column17" headerRowDxfId="117" dataDxfId="116"/>
+    <tableColumn id="1" xr3:uid="{A5B7E7CC-F2E9-4C49-BED9-3A47CAE54B7E}" name="Column1" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{1F4A7765-A904-4DF6-B648-094B6BC94FBE}" name="Column2" headerRowDxfId="149" dataDxfId="148"/>
+    <tableColumn id="3" xr3:uid="{839ADCF5-8C6D-4A0C-AAB2-969A42AE8027}" name="Column3" headerRowDxfId="147" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{1731EB37-AE35-486E-855D-77128F4DDF09}" name="Column4" headerRowDxfId="145" dataDxfId="144"/>
+    <tableColumn id="5" xr3:uid="{4F3895B0-C799-4B3D-8759-283BB22EA08E}" name="Column5" headerRowDxfId="143" dataDxfId="142"/>
+    <tableColumn id="6" xr3:uid="{31207C71-AA84-443E-824A-E507F7192E3F}" name="Column6" headerRowDxfId="141" dataDxfId="140"/>
+    <tableColumn id="7" xr3:uid="{3D4AA28B-3E08-4F46-B50A-0C65CF425433}" name="Column7" headerRowDxfId="139" dataDxfId="138"/>
+    <tableColumn id="8" xr3:uid="{64223BBE-3219-453E-AD2C-61C0B9A09904}" name="Column8" headerRowDxfId="137" dataDxfId="136"/>
+    <tableColumn id="9" xr3:uid="{11687BFD-11FB-41C8-B4D4-CDB9E0136019}" name="Column9" headerRowDxfId="135" dataDxfId="134"/>
+    <tableColumn id="10" xr3:uid="{7EF49BEB-C450-4CDD-A592-0945074DF1B6}" name="Column10" headerRowDxfId="133" dataDxfId="132"/>
+    <tableColumn id="11" xr3:uid="{AAA731DE-3024-44C5-83DB-F983987C19BD}" name="Column11" headerRowDxfId="131" dataDxfId="130"/>
+    <tableColumn id="12" xr3:uid="{C2E61F83-831E-4409-9DD2-49A133F6632F}" name="Column12" headerRowDxfId="129" dataDxfId="128"/>
+    <tableColumn id="13" xr3:uid="{36F29327-806B-4BFE-98EF-D858E1BE52B2}" name="Column13" headerRowDxfId="127" dataDxfId="126"/>
+    <tableColumn id="14" xr3:uid="{BAE00B6F-FE30-4E85-AD72-BA5846AF950C}" name="Column14" headerRowDxfId="125" dataDxfId="124"/>
+    <tableColumn id="15" xr3:uid="{56476BC5-A36D-4837-8C13-38FEA912BAC5}" name="Column15" headerRowDxfId="123" dataDxfId="122"/>
+    <tableColumn id="16" xr3:uid="{1C4EAA2A-CB75-4A15-87A1-9CDC9F820B8C}" name="Column16" headerRowDxfId="121" dataDxfId="120"/>
+    <tableColumn id="17" xr3:uid="{C9171481-5E79-493E-A3D8-98929F6931FC}" name="Column17" headerRowDxfId="119" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{29BE427D-AEEF-43FD-9197-5BC12488B6A0}" name="pointscalculator_division3" displayName="pointscalculator_division3" ref="D39:T52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{29BE427D-AEEF-43FD-9197-5BC12488B6A0}" name="pointscalculator_division3" displayName="pointscalculator_division3" ref="D39:T52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{FC4A3AA2-2C15-4A4D-A0B1-390B1DB00E83}" name="Column1" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{C31EA6F2-0FBC-4840-B86F-FF5C35E4C28C}" name="Column2" headerRowDxfId="112" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{3AFE98A5-75F5-41CB-B1EC-49E614C87BF0}" name="Column3" headerRowDxfId="110" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{48E7C085-8DFF-457A-BB2E-C6F1B98CD806}" name="Column4" headerRowDxfId="108" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{CB53D151-239B-4449-90A9-7A45D7A24982}" name="Column5" headerRowDxfId="106" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{BF1A98FD-3CA4-4E00-99CD-95C07EE77E29}" name="Column6" headerRowDxfId="104" dataDxfId="103"/>
-    <tableColumn id="7" xr3:uid="{AAC9C9E9-A170-4DF4-A5E4-5DC08E69350B}" name="Column7" headerRowDxfId="102" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{0F098E18-2618-40F7-B7F5-A2C2726A73ED}" name="Column8" headerRowDxfId="100" dataDxfId="99"/>
-    <tableColumn id="9" xr3:uid="{DD100799-1EDD-48D5-A652-83C8A28D3E9C}" name="Column9" headerRowDxfId="98" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{3B30BFB9-5C90-4BEE-A4A5-25DE6F3AF3C6}" name="Column10" headerRowDxfId="96" dataDxfId="95"/>
-    <tableColumn id="11" xr3:uid="{8A9DB7F8-2B58-46BC-9C54-E70EB7C0A43B}" name="Column11" headerRowDxfId="94" dataDxfId="93"/>
-    <tableColumn id="12" xr3:uid="{7AF033F3-1D1E-46DB-B11A-BD277D16B337}" name="Column12" headerRowDxfId="92" dataDxfId="91"/>
-    <tableColumn id="13" xr3:uid="{ED2F8951-0A3F-41AC-B1B1-A8A039DD18BE}" name="Column13" headerRowDxfId="90" dataDxfId="89"/>
-    <tableColumn id="14" xr3:uid="{5EDC0120-BC0F-4485-80FB-2F85953C0A27}" name="Column14" headerRowDxfId="88" dataDxfId="87"/>
-    <tableColumn id="15" xr3:uid="{2F54CDE7-8BD4-4B75-A942-9CC6465B1740}" name="Column15" headerRowDxfId="86" dataDxfId="85"/>
-    <tableColumn id="16" xr3:uid="{BD867E6D-8DFD-45E7-8ED3-2FE76F68C835}" name="Column16" headerRowDxfId="84" dataDxfId="83"/>
-    <tableColumn id="17" xr3:uid="{D8E98697-97CE-4ACD-A41D-EDB9B5F2BD4E}" name="Column17" headerRowDxfId="82" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{FC4A3AA2-2C15-4A4D-A0B1-390B1DB00E83}" name="Column1" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{C31EA6F2-0FBC-4840-B86F-FF5C35E4C28C}" name="Column2" headerRowDxfId="114" dataDxfId="113"/>
+    <tableColumn id="3" xr3:uid="{3AFE98A5-75F5-41CB-B1EC-49E614C87BF0}" name="Column3" headerRowDxfId="112" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{48E7C085-8DFF-457A-BB2E-C6F1B98CD806}" name="Column4" headerRowDxfId="110" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{CB53D151-239B-4449-90A9-7A45D7A24982}" name="Column5" headerRowDxfId="108" dataDxfId="107"/>
+    <tableColumn id="6" xr3:uid="{BF1A98FD-3CA4-4E00-99CD-95C07EE77E29}" name="Column6" headerRowDxfId="106" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{AAC9C9E9-A170-4DF4-A5E4-5DC08E69350B}" name="Column7" headerRowDxfId="104" dataDxfId="103"/>
+    <tableColumn id="8" xr3:uid="{0F098E18-2618-40F7-B7F5-A2C2726A73ED}" name="Column8" headerRowDxfId="102" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{DD100799-1EDD-48D5-A652-83C8A28D3E9C}" name="Column9" headerRowDxfId="100" dataDxfId="99"/>
+    <tableColumn id="10" xr3:uid="{3B30BFB9-5C90-4BEE-A4A5-25DE6F3AF3C6}" name="Column10" headerRowDxfId="98" dataDxfId="97"/>
+    <tableColumn id="11" xr3:uid="{8A9DB7F8-2B58-46BC-9C54-E70EB7C0A43B}" name="Column11" headerRowDxfId="96" dataDxfId="95"/>
+    <tableColumn id="12" xr3:uid="{7AF033F3-1D1E-46DB-B11A-BD277D16B337}" name="Column12" headerRowDxfId="94" dataDxfId="93"/>
+    <tableColumn id="13" xr3:uid="{ED2F8951-0A3F-41AC-B1B1-A8A039DD18BE}" name="Column13" headerRowDxfId="92" dataDxfId="91"/>
+    <tableColumn id="14" xr3:uid="{5EDC0120-BC0F-4485-80FB-2F85953C0A27}" name="Column14" headerRowDxfId="90" dataDxfId="89"/>
+    <tableColumn id="15" xr3:uid="{2F54CDE7-8BD4-4B75-A942-9CC6465B1740}" name="Column15" headerRowDxfId="88" dataDxfId="87"/>
+    <tableColumn id="16" xr3:uid="{BD867E6D-8DFD-45E7-8ED3-2FE76F68C835}" name="Column16" headerRowDxfId="86" dataDxfId="85"/>
+    <tableColumn id="17" xr3:uid="{D8E98697-97CE-4ACD-A41D-EDB9B5F2BD4E}" name="Column17" headerRowDxfId="84" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A07179E9-6376-4F82-A951-1C094AAE9248}" name="pointscalculator_division0" displayName="pointscalculator_division0" ref="D57:T70" headerRowCount="0" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A07179E9-6376-4F82-A951-1C094AAE9248}" name="pointscalculator_division0" displayName="pointscalculator_division0" ref="D57:T70" headerRowCount="0" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E8193783-C27A-431A-9572-AFA00587EF56}" name="Column1" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{3269A5B5-EA59-431E-BF9E-6C54925FF873}" name="Column2" headerRowDxfId="77" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{D68A4479-C625-483F-8606-D5D58D70CA92}" name="Column3" headerRowDxfId="75" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{B7951688-6C6E-488C-9FCD-62063D8E1B8F}" name="Column4" headerRowDxfId="73" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{3E2FCED4-3293-4733-918D-9A21E583BB3A}" name="Column5" headerRowDxfId="71" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{BE3DF187-D34F-44CC-B9D2-6974955E38C9}" name="Column6" headerRowDxfId="69" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{5216B523-4E53-47AC-96C4-5A425B7E0549}" name="Column7" headerRowDxfId="67" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{34633752-5250-4B0B-B176-38CFBA6F28C8}" name="Column8" headerRowDxfId="65" dataDxfId="64"/>
-    <tableColumn id="9" xr3:uid="{CE238B24-303C-4362-9B47-B981AAAE0F84}" name="Column9" headerRowDxfId="63" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{F3251511-0A59-4269-8CC5-746E6365054C}" name="Column10" headerRowDxfId="61" dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{424312CA-02E5-4EC0-A003-334CC04EE9D2}" name="Column11" headerRowDxfId="59" dataDxfId="58"/>
-    <tableColumn id="12" xr3:uid="{0F5AC330-BD38-4A40-A538-ED741C233178}" name="Column12" headerRowDxfId="57" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{55915551-1C82-408B-80C7-E3512638D8B1}" name="Column13" headerRowDxfId="55" dataDxfId="54"/>
-    <tableColumn id="14" xr3:uid="{9CCB53C7-C0C9-4350-B68D-6F5E87DE5F4C}" name="Column14" headerRowDxfId="53" dataDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{785CADF6-753C-4FE7-9311-3D5E85CAA8D0}" name="Column15" headerRowDxfId="51" dataDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{EB97894A-1F48-477B-94E2-CBA9CA249DFF}" name="Column16" headerRowDxfId="49" dataDxfId="48"/>
-    <tableColumn id="17" xr3:uid="{2F00A99B-5728-43AF-A412-6250E56BA1B3}" name="Column17" headerRowDxfId="47" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{E8193783-C27A-431A-9572-AFA00587EF56}" name="Column1" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{3269A5B5-EA59-431E-BF9E-6C54925FF873}" name="Column2" headerRowDxfId="79" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{D68A4479-C625-483F-8606-D5D58D70CA92}" name="Column3" headerRowDxfId="77" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{B7951688-6C6E-488C-9FCD-62063D8E1B8F}" name="Column4" headerRowDxfId="75" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{3E2FCED4-3293-4733-918D-9A21E583BB3A}" name="Column5" headerRowDxfId="73" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{BE3DF187-D34F-44CC-B9D2-6974955E38C9}" name="Column6" headerRowDxfId="71" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{5216B523-4E53-47AC-96C4-5A425B7E0549}" name="Column7" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="8" xr3:uid="{34633752-5250-4B0B-B176-38CFBA6F28C8}" name="Column8" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{CE238B24-303C-4362-9B47-B981AAAE0F84}" name="Column9" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{F3251511-0A59-4269-8CC5-746E6365054C}" name="Column10" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{424312CA-02E5-4EC0-A003-334CC04EE9D2}" name="Column11" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{0F5AC330-BD38-4A40-A538-ED741C233178}" name="Column12" headerRowDxfId="59" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{55915551-1C82-408B-80C7-E3512638D8B1}" name="Column13" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{9CCB53C7-C0C9-4350-B68D-6F5E87DE5F4C}" name="Column14" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="15" xr3:uid="{785CADF6-753C-4FE7-9311-3D5E85CAA8D0}" name="Column15" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{EB97894A-1F48-477B-94E2-CBA9CA249DFF}" name="Column16" headerRowDxfId="51" dataDxfId="50"/>
+    <tableColumn id="17" xr3:uid="{2F00A99B-5728-43AF-A412-6250E56BA1B3}" name="Column17" headerRowDxfId="49" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C066228F-627D-45C1-9355-45199E7024A2}" name="Karts_division1101223" displayName="Karts_division1101223" ref="A1:E15" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C066228F-627D-45C1-9355-45199E7024A2}" name="Karts_division1101223" displayName="Karts_division1101223" ref="A1:E15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{499ED437-E2A3-4DEB-9BE1-88FED55AA0D4}" name="Kart #" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{2ED3F931-9976-4869-9697-DFB0578B06A9}" name="Average Time" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{0CA1B145-AB78-4B49-B984-82824F8E6A64}" name="Best Time" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{61238CAE-31CA-4F7B-B7CA-C34249324F70}" name="Name" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{638B4A1A-D3FB-456A-8196-3FE015470B50}" name="Start" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{499ED437-E2A3-4DEB-9BE1-88FED55AA0D4}" name="Kart #" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{2ED3F931-9976-4869-9697-DFB0578B06A9}" name="Average Time" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{0CA1B145-AB78-4B49-B984-82824F8E6A64}" name="Best Time" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{61238CAE-31CA-4F7B-B7CA-C34249324F70}" name="Name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{638B4A1A-D3FB-456A-8196-3FE015470B50}" name="Start" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{A7B10B46-A422-41FE-867F-3C32FDD82113}" name="kartpick_division1112224" displayName="kartpick_division1112224" ref="I1:J15" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{A7B10B46-A422-41FE-867F-3C32FDD82113}" name="kartpick_division1112224" displayName="kartpick_division1112224" ref="I1:J15" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A3B373D5-2CE5-4D66-8EF5-A96407FE0F68}" name="Name" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{A3B373D5-2CE5-4D66-8EF5-A96407FE0F68}" name="Name" dataDxfId="1">
       <calculatedColumnFormula>Roster!I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E06DD3EE-C704-4E82-9776-DEC1BF9920B9}" name="Weight" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{E06DD3EE-C704-4E82-9776-DEC1BF9920B9}" name="Weight" dataDxfId="0">
       <calculatedColumnFormula>Roster!K4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2585,30 +2599,30 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}" name="Karts_division1" displayName="Karts_division1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}" name="Karts_division1" displayName="Karts_division1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2F48F510-80F4-438B-9709-8408B51A9904}" name="Kart #" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{B77A82F5-DEA1-428E-9E9F-7C6DD69D0486}" name="Average Time"/>
-    <tableColumn id="3" xr3:uid="{B07CD94E-7ED1-4DE3-8E56-A36E6E39070A}" name="Best Time"/>
-    <tableColumn id="4" xr3:uid="{F63BEB9B-0159-46AB-AAF5-42323633C103}" name="Name" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{85ED9692-6A48-4689-9A9B-00533CD29B14}" name="Start" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{2F48F510-80F4-438B-9709-8408B51A9904}" name="Kart #" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{B77A82F5-DEA1-428E-9E9F-7C6DD69D0486}" name="Average Time" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B07CD94E-7ED1-4DE3-8E56-A36E6E39070A}" name="Best Time" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{F63BEB9B-0159-46AB-AAF5-42323633C103}" name="Name" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{85ED9692-6A48-4689-9A9B-00533CD29B14}" name="Start" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}" name="kartpick_division1" displayName="kartpick_division1" ref="I1:J15" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}" name="kartpick_division1" displayName="kartpick_division1" ref="I1:J15" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F708E8BD-68A5-4939-B036-1CE26E2016B1}" name="Name" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{F708E8BD-68A5-4939-B036-1CE26E2016B1}" name="Name" dataDxfId="8">
       <calculatedColumnFormula>Roster!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B4A6FAAD-26D9-4845-ABD2-AB0AF2BF0338}" name="Weight" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{B4A6FAAD-26D9-4845-ABD2-AB0AF2BF0338}" name="Weight" dataDxfId="7">
       <calculatedColumnFormula>Roster!C4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2617,36 +2631,36 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5E0827B4-9E05-452D-8784-07C4744F9A8E}" name="Karts_division110" displayName="Karts_division110" ref="A1:E15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5E0827B4-9E05-452D-8784-07C4744F9A8E}" name="Karts_division110" displayName="Karts_division110" ref="A1:E15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0B02D3BA-ECCE-428F-808D-F7CEE48D79D5}" name="Kart #" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{0B02D3BA-ECCE-428F-808D-F7CEE48D79D5}" name="Kart #" dataDxfId="19">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Kart '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{61B2FC20-6361-4065-B02C-493401236E59}" name="Average Time" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{61B2FC20-6361-4065-B02C-493401236E59}" name="Average Time" dataDxfId="18">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Average Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C58B34E1-8D68-4A3F-871A-CE737B90914D}" name="Best Time" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{C58B34E1-8D68-4A3F-871A-CE737B90914D}" name="Best Time" dataDxfId="17">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Best Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{90EDB97E-D031-451E-94B0-18EC0C56E099}" name="Name" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{D266CDBD-0214-4C1D-A8A8-15F3D652F0D8}" name="Start" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{90EDB97E-D031-451E-94B0-18EC0C56E099}" name="Name" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{D266CDBD-0214-4C1D-A8A8-15F3D652F0D8}" name="Start" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDC6AC44-B1CE-4FBC-A9AD-41D438DD98D9}" name="kartpick_division111" displayName="kartpick_division111" ref="I1:J15" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDC6AC44-B1CE-4FBC-A9AD-41D438DD98D9}" name="kartpick_division111" displayName="kartpick_division111" ref="I1:J15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3BCE534D-806A-4501-ADC4-EB317288D00D}" name="Name" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{3BCE534D-806A-4501-ADC4-EB317288D00D}" name="Name" dataDxfId="12">
       <calculatedColumnFormula>Roster!E4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5570B562-4FDC-4E2A-97EA-18DE8E46A7EC}" name="Weight" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{5570B562-4FDC-4E2A-97EA-18DE8E46A7EC}" name="Weight" dataDxfId="11">
       <calculatedColumnFormula>Roster!G4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2655,48 +2669,48 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7D1EA9C5-2067-40EA-8B4E-B5F935E0FB53}" name="roster_division2" displayName="roster_division2" ref="E3:G15" totalsRowShown="0" headerRowDxfId="255" dataDxfId="254">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7D1EA9C5-2067-40EA-8B4E-B5F935E0FB53}" name="roster_division2" displayName="roster_division2" ref="E3:G15" totalsRowShown="0" headerRowDxfId="257" dataDxfId="256">
   <autoFilter ref="E3:G15" xr:uid="{7D1EA9C5-2067-40EA-8B4E-B5F935E0FB53}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4FFFCFAA-FAD8-40C1-863E-091C6E432A67}" name="First Name" dataDxfId="253"/>
-    <tableColumn id="2" xr3:uid="{19F1D3EA-A312-4D66-B515-80A54F1AA0E4}" name="Last Name" dataDxfId="252"/>
-    <tableColumn id="3" xr3:uid="{076A1852-2D63-48B9-8597-066387E0C88D}" name="Weight" dataDxfId="251"/>
+    <tableColumn id="1" xr3:uid="{4FFFCFAA-FAD8-40C1-863E-091C6E432A67}" name="First Name" dataDxfId="255"/>
+    <tableColumn id="2" xr3:uid="{19F1D3EA-A312-4D66-B515-80A54F1AA0E4}" name="Last Name" dataDxfId="254"/>
+    <tableColumn id="3" xr3:uid="{076A1852-2D63-48B9-8597-066387E0C88D}" name="Weight" dataDxfId="253"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D7B5CB3-DF61-402A-8F35-D46CBBAF2AC3}" name="Karts_division11012" displayName="Karts_division11012" ref="A1:E15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D7B5CB3-DF61-402A-8F35-D46CBBAF2AC3}" name="Karts_division11012" displayName="Karts_division11012" ref="A1:E15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60522C3F-A4DF-4A38-81FF-1E9B1C221E03}" name="Kart #" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{60522C3F-A4DF-4A38-81FF-1E9B1C221E03}" name="Kart #" dataDxfId="30">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Kart '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EC9933E0-4869-42D9-9C24-3AE08EEC4D7A}" name="Average Time" dataDxfId="11">
+    <tableColumn id="2" xr3:uid="{EC9933E0-4869-42D9-9C24-3AE08EEC4D7A}" name="Average Time" dataDxfId="29">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Average Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{85CAC5CF-E710-40E2-8635-6F4A05E7ECB2}" name="Best Time" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{85CAC5CF-E710-40E2-8635-6F4A05E7ECB2}" name="Best Time" dataDxfId="28">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Best Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4D4EEBB5-2C21-4DE9-B095-29000447CD26}" name="Name" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{F70CFA25-DC14-45B1-9EE0-4182384834AC}" name="Start" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4D4EEBB5-2C21-4DE9-B095-29000447CD26}" name="Name" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F70CFA25-DC14-45B1-9EE0-4182384834AC}" name="Start" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C94D2B82-0FF7-449F-A200-F6F1EBEDFD14}" name="kartpick_division11122" displayName="kartpick_division11122" ref="I1:J15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C94D2B82-0FF7-449F-A200-F6F1EBEDFD14}" name="kartpick_division11122" displayName="kartpick_division11122" ref="I1:J15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{268D7F68-EB66-467B-89AA-B6037DB21EFE}" name="Name" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{268D7F68-EB66-467B-89AA-B6037DB21EFE}" name="Name" dataDxfId="23">
       <calculatedColumnFormula>Roster!I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D6A8D05A-702B-41AB-BD0F-2BE11F778C3C}" name="Weight" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{D6A8D05A-702B-41AB-BD0F-2BE11F778C3C}" name="Weight" dataDxfId="22">
       <calculatedColumnFormula>Roster!K4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2705,64 +2719,64 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{471D2A0A-D58F-49AB-93A5-8B48010C5429}" name="roster_division3" displayName="roster_division3" ref="I3:K15" totalsRowShown="0" headerRowDxfId="250" dataDxfId="249">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{471D2A0A-D58F-49AB-93A5-8B48010C5429}" name="roster_division3" displayName="roster_division3" ref="I3:K15" totalsRowShown="0" headerRowDxfId="252" dataDxfId="251">
   <autoFilter ref="I3:K15" xr:uid="{471D2A0A-D58F-49AB-93A5-8B48010C5429}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A57067-6DA5-4E1D-AD82-EC63961B32E2}" name="First Name" dataDxfId="248"/>
-    <tableColumn id="2" xr3:uid="{CDB5ADB5-132A-4E3A-B782-E6D87E861173}" name="Last Name" dataDxfId="247"/>
-    <tableColumn id="3" xr3:uid="{B161C779-62FA-4ED7-B06D-6EC3DC591180}" name="Weight" dataDxfId="246"/>
+    <tableColumn id="1" xr3:uid="{50A57067-6DA5-4E1D-AD82-EC63961B32E2}" name="First Name" dataDxfId="250"/>
+    <tableColumn id="2" xr3:uid="{CDB5ADB5-132A-4E3A-B782-E6D87E861173}" name="Last Name" dataDxfId="249"/>
+    <tableColumn id="3" xr3:uid="{B161C779-62FA-4ED7-B06D-6EC3DC591180}" name="Weight" dataDxfId="248"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{72C84625-5679-468F-A862-90642D885CDC}" name="roster_division0" displayName="roster_division0" ref="M3:O15" totalsRowShown="0" headerRowDxfId="245" dataDxfId="244">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{72C84625-5679-468F-A862-90642D885CDC}" name="roster_division0" displayName="roster_division0" ref="M3:O15" totalsRowShown="0" headerRowDxfId="247" dataDxfId="246">
   <autoFilter ref="M3:O15" xr:uid="{72C84625-5679-468F-A862-90642D885CDC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6AD26058-4C29-4FBC-816F-8E2D06847E15}" name="First Name" dataDxfId="243"/>
-    <tableColumn id="2" xr3:uid="{0116F307-4EBB-431D-8D34-C71E53721D82}" name="Last Name" dataDxfId="242"/>
-    <tableColumn id="3" xr3:uid="{27132D2A-F787-4D1E-B8AC-4A920907B6B1}" name="Weight" dataDxfId="241"/>
+    <tableColumn id="1" xr3:uid="{6AD26058-4C29-4FBC-816F-8E2D06847E15}" name="First Name" dataDxfId="245"/>
+    <tableColumn id="2" xr3:uid="{0116F307-4EBB-431D-8D34-C71E53721D82}" name="Last Name" dataDxfId="244"/>
+    <tableColumn id="3" xr3:uid="{27132D2A-F787-4D1E-B8AC-4A920907B6B1}" name="Weight" dataDxfId="243"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}" name="leaderboard_division1" displayName="leaderboard_division1" ref="A3:J15" totalsRowShown="0" headerRowDxfId="240" dataDxfId="239">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}" name="leaderboard_division1" displayName="leaderboard_division1" ref="A3:J15" totalsRowShown="0" headerRowDxfId="242" dataDxfId="241">
   <autoFilter ref="A3:J15" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J15">
     <sortCondition descending="1" ref="J3:J15"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3EE385B5-186A-494C-99F2-4DA44BADE713}" name="Name" dataDxfId="238">
+    <tableColumn id="1" xr3:uid="{3EE385B5-186A-494C-99F2-4DA44BADE713}" name="Name" dataDxfId="240">
       <calculatedColumnFormula>CONCATENATE(Roster!A4, " ", Roster!B4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{05CFC75F-5D8B-4EC9-BE8F-7645475F318F}" name="Week 1" dataDxfId="237">
+    <tableColumn id="2" xr3:uid="{05CFC75F-5D8B-4EC9-BE8F-7645475F318F}" name="Week 1" dataDxfId="239">
       <calculatedColumnFormula>'Points calculator'!F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{27DA45F0-FBF3-41F0-89C5-3D9C04B59601}" name="Week 2" dataDxfId="236">
+    <tableColumn id="3" xr3:uid="{27DA45F0-FBF3-41F0-89C5-3D9C04B59601}" name="Week 2" dataDxfId="238">
       <calculatedColumnFormula>'Points calculator'!H5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1FB2A630-4026-4BD5-AB32-3BABB3917000}" name="Week 3" dataDxfId="235">
+    <tableColumn id="4" xr3:uid="{1FB2A630-4026-4BD5-AB32-3BABB3917000}" name="Week 3" dataDxfId="237">
       <calculatedColumnFormula>'Points calculator'!J5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{477B59BB-336A-42CA-B49A-D66E72883C9D}" name="Week 4" dataDxfId="234">
+    <tableColumn id="5" xr3:uid="{477B59BB-336A-42CA-B49A-D66E72883C9D}" name="Week 4" dataDxfId="236">
       <calculatedColumnFormula>'Points calculator'!K5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D41E8B54-8B08-47BE-BFC4-3D5D584C943B}" name="Week 5" dataDxfId="233">
+    <tableColumn id="6" xr3:uid="{D41E8B54-8B08-47BE-BFC4-3D5D584C943B}" name="Week 5" dataDxfId="235">
       <calculatedColumnFormula>'Points calculator'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{42081221-B4AD-4019-8EBD-DDABA83F2B96}" name="Week 6" dataDxfId="232">
+    <tableColumn id="7" xr3:uid="{42081221-B4AD-4019-8EBD-DDABA83F2B96}" name="Week 6" dataDxfId="234">
       <calculatedColumnFormula>'Points calculator'!O5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{51CDE54B-C103-49F1-934C-7FB5B7C950BB}" name="Week 7" dataDxfId="231">
+    <tableColumn id="8" xr3:uid="{51CDE54B-C103-49F1-934C-7FB5B7C950BB}" name="Week 7" dataDxfId="233">
       <calculatedColumnFormula>'Points calculator'!Q5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{456B5849-E8D5-4C55-879E-90997FD8604B}" name="Week 8" dataDxfId="230">
+    <tableColumn id="9" xr3:uid="{456B5849-E8D5-4C55-879E-90997FD8604B}" name="Week 8" dataDxfId="232">
       <calculatedColumnFormula>'Points calculator'!R5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6DACC5D1-5115-470B-87C2-D8F58FFB46DE}" name="Total" dataDxfId="229">
+    <tableColumn id="10" xr3:uid="{6DACC5D1-5115-470B-87C2-D8F58FFB46DE}" name="Total" dataDxfId="231">
       <calculatedColumnFormula>SUM(B4:I4) - MIN(B4:I4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2771,40 +2785,40 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}" name="leaderboard_division2" displayName="leaderboard_division2" ref="A20:J32" totalsRowShown="0" headerRowDxfId="228" dataDxfId="227">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}" name="leaderboard_division2" displayName="leaderboard_division2" ref="A20:J32" totalsRowShown="0" headerRowDxfId="230" dataDxfId="229">
   <autoFilter ref="A20:J32" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:J32">
     <sortCondition descending="1" ref="J20:J32"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8920F168-081D-48F4-B861-3BF464DCB24E}" name="Name" dataDxfId="226">
+    <tableColumn id="1" xr3:uid="{8920F168-081D-48F4-B861-3BF464DCB24E}" name="Name" dataDxfId="228">
       <calculatedColumnFormula>CONCATENATE(Roster!E4, " ", Roster!F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1FB66D7A-AD86-40F5-A827-6FD25FC3711D}" name="Week 1" dataDxfId="225">
+    <tableColumn id="2" xr3:uid="{1FB66D7A-AD86-40F5-A827-6FD25FC3711D}" name="Week 1" dataDxfId="227">
       <calculatedColumnFormula>'Points calculator'!F23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1347C6E6-6BCB-42E7-9A6C-7EEEBF3112D3}" name="Week 2" dataDxfId="224">
+    <tableColumn id="3" xr3:uid="{1347C6E6-6BCB-42E7-9A6C-7EEEBF3112D3}" name="Week 2" dataDxfId="226">
       <calculatedColumnFormula>'Points calculator'!H23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B834E847-A249-4368-BE53-6EBA45B7B65C}" name="Week 3" dataDxfId="223">
+    <tableColumn id="4" xr3:uid="{B834E847-A249-4368-BE53-6EBA45B7B65C}" name="Week 3" dataDxfId="225">
       <calculatedColumnFormula>'Points calculator'!J23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{842CDE93-7EC7-486C-AA50-AFA1DACADDE2}" name="Week 4" dataDxfId="222">
+    <tableColumn id="5" xr3:uid="{842CDE93-7EC7-486C-AA50-AFA1DACADDE2}" name="Week 4" dataDxfId="224">
       <calculatedColumnFormula>'Points calculator'!K23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0F38C0C3-9F35-46B2-B0E8-5C9089A436D9}" name="Week 5" dataDxfId="221">
+    <tableColumn id="6" xr3:uid="{0F38C0C3-9F35-46B2-B0E8-5C9089A436D9}" name="Week 5" dataDxfId="223">
       <calculatedColumnFormula>'Points calculator'!M23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E1BEDA47-31FA-4364-AD3B-6C89ED4E973E}" name="Week 6" dataDxfId="220">
+    <tableColumn id="7" xr3:uid="{E1BEDA47-31FA-4364-AD3B-6C89ED4E973E}" name="Week 6" dataDxfId="222">
       <calculatedColumnFormula>'Points calculator'!O23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8858DDC5-2FC3-484A-ABC1-8D968F1ADF71}" name="Week 7" dataDxfId="219">
+    <tableColumn id="8" xr3:uid="{8858DDC5-2FC3-484A-ABC1-8D968F1ADF71}" name="Week 7" dataDxfId="221">
       <calculatedColumnFormula>'Points calculator'!Q23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D71C639C-9F32-4C45-A01C-8AEAD864E7DB}" name="Week 8" dataDxfId="218">
+    <tableColumn id="9" xr3:uid="{D71C639C-9F32-4C45-A01C-8AEAD864E7DB}" name="Week 8" dataDxfId="220">
       <calculatedColumnFormula>'Points calculator'!R23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DA5645D4-E081-4931-84D9-D7D83BD8A055}" name="Total" dataDxfId="217">
+    <tableColumn id="10" xr3:uid="{DA5645D4-E081-4931-84D9-D7D83BD8A055}" name="Total" dataDxfId="219">
       <calculatedColumnFormula>SUM(B21:I21) - MIN(B21:I21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2813,40 +2827,40 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}" name="leaderboard_division3" displayName="leaderboard_division3" ref="M3:V15" totalsRowShown="0" headerRowDxfId="216" dataDxfId="215">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}" name="leaderboard_division3" displayName="leaderboard_division3" ref="M3:V15" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217">
   <autoFilter ref="M3:V15" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:V15">
     <sortCondition descending="1" ref="V3:V15"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{24729B62-D12C-44C0-A782-2B723A80950C}" name="Name" dataDxfId="214">
+    <tableColumn id="1" xr3:uid="{24729B62-D12C-44C0-A782-2B723A80950C}" name="Name" dataDxfId="216">
       <calculatedColumnFormula>CONCATENATE(roster_division3[[#This Row],[First Name]], " ", roster_division3[[#This Row],[Last Name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E2C19456-E2D6-4570-AAAC-F16C54F47CF2}" name="Week 1" dataDxfId="213">
+    <tableColumn id="2" xr3:uid="{E2C19456-E2D6-4570-AAAC-F16C54F47CF2}" name="Week 1" dataDxfId="215">
       <calculatedColumnFormula>'Points calculator'!F41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{003D5C38-C0D2-42E9-A987-6CFB7A7EB4C6}" name="Week 2" dataDxfId="212">
+    <tableColumn id="3" xr3:uid="{003D5C38-C0D2-42E9-A987-6CFB7A7EB4C6}" name="Week 2" dataDxfId="214">
       <calculatedColumnFormula>'Points calculator'!H41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AC94F960-BB0C-4A06-86A2-5ACDAFADAC89}" name="Week 3" dataDxfId="211">
+    <tableColumn id="4" xr3:uid="{AC94F960-BB0C-4A06-86A2-5ACDAFADAC89}" name="Week 3" dataDxfId="213">
       <calculatedColumnFormula>'Points calculator'!J41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F9D774A5-F6E6-4242-841D-7AF4A28B2DF0}" name="Week 4" dataDxfId="210">
+    <tableColumn id="5" xr3:uid="{F9D774A5-F6E6-4242-841D-7AF4A28B2DF0}" name="Week 4" dataDxfId="212">
       <calculatedColumnFormula>'Points calculator'!K41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EFBBCB3A-63C3-4BDD-9BE2-08298E219562}" name="Week 5" dataDxfId="209">
+    <tableColumn id="6" xr3:uid="{EFBBCB3A-63C3-4BDD-9BE2-08298E219562}" name="Week 5" dataDxfId="211">
       <calculatedColumnFormula>'Points calculator'!M41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A547CC97-7F1A-45D2-94F5-2DE2E6BEF78A}" name="Week 6" dataDxfId="208">
+    <tableColumn id="7" xr3:uid="{A547CC97-7F1A-45D2-94F5-2DE2E6BEF78A}" name="Week 6" dataDxfId="210">
       <calculatedColumnFormula>'Points calculator'!O41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5DBCD7BF-BD88-421F-99C9-3FAAE459C430}" name="Week 7" dataDxfId="207">
+    <tableColumn id="8" xr3:uid="{5DBCD7BF-BD88-421F-99C9-3FAAE459C430}" name="Week 7" dataDxfId="209">
       <calculatedColumnFormula>'Points calculator'!Q41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8054E0E9-7986-4AED-8C91-466FA9652580}" name="Week 8" dataDxfId="206">
+    <tableColumn id="9" xr3:uid="{8054E0E9-7986-4AED-8C91-466FA9652580}" name="Week 8" dataDxfId="208">
       <calculatedColumnFormula>'Points calculator'!R41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C70C4803-97FF-4296-A9D8-829CA80E97B4}" name="Total" dataDxfId="205">
+    <tableColumn id="10" xr3:uid="{C70C4803-97FF-4296-A9D8-829CA80E97B4}" name="Total" dataDxfId="207">
       <calculatedColumnFormula>SUM(N4:U4) - MIN(N4:U4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2855,40 +2869,40 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}" name="leaderboard_division0" displayName="leaderboard_division0" ref="M20:V32" totalsRowShown="0" headerRowDxfId="204" dataDxfId="203">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}" name="leaderboard_division0" displayName="leaderboard_division0" ref="M20:V32" totalsRowShown="0" headerRowDxfId="206" dataDxfId="205">
   <autoFilter ref="M20:V32" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M21:V32">
     <sortCondition descending="1" ref="V20:V32"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F5489658-A403-4D4D-8477-63F70A31236F}" name="Name" dataDxfId="202">
+    <tableColumn id="1" xr3:uid="{F5489658-A403-4D4D-8477-63F70A31236F}" name="Name" dataDxfId="204">
       <calculatedColumnFormula>CONCATENATE(Roster!M4, " ", Roster!N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5274554A-7441-4132-9B00-0EB064D33B2E}" name="Week 1" dataDxfId="201">
+    <tableColumn id="2" xr3:uid="{5274554A-7441-4132-9B00-0EB064D33B2E}" name="Week 1" dataDxfId="203">
       <calculatedColumnFormula>'Points calculator'!F59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9575F9E7-CA68-4FE1-8BD8-120189BF05FB}" name="Week 2" dataDxfId="200">
+    <tableColumn id="3" xr3:uid="{9575F9E7-CA68-4FE1-8BD8-120189BF05FB}" name="Week 2" dataDxfId="202">
       <calculatedColumnFormula>'Points calculator'!H59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D8C8B55B-2A0D-49B7-A9AB-F098FBEE9986}" name="Week 3" dataDxfId="199">
+    <tableColumn id="4" xr3:uid="{D8C8B55B-2A0D-49B7-A9AB-F098FBEE9986}" name="Week 3" dataDxfId="201">
       <calculatedColumnFormula>'Points calculator'!J59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4ACB5F81-948D-42B6-BFFE-92CED40E0588}" name="Week 4" dataDxfId="198">
+    <tableColumn id="5" xr3:uid="{4ACB5F81-948D-42B6-BFFE-92CED40E0588}" name="Week 4" dataDxfId="200">
       <calculatedColumnFormula>'Points calculator'!K59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3554C417-4367-4989-8FD7-D5D934DE290B}" name="Week 5" dataDxfId="197">
+    <tableColumn id="6" xr3:uid="{3554C417-4367-4989-8FD7-D5D934DE290B}" name="Week 5" dataDxfId="199">
       <calculatedColumnFormula>'Points calculator'!M59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2F5C655-EB8A-4B84-8838-3144A89DFFB7}" name="Week 6" dataDxfId="196">
+    <tableColumn id="7" xr3:uid="{E2F5C655-EB8A-4B84-8838-3144A89DFFB7}" name="Week 6" dataDxfId="198">
       <calculatedColumnFormula>'Points calculator'!O59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7179BFAD-F782-439F-BB1D-7249215D9DD8}" name="Week 7" dataDxfId="195">
+    <tableColumn id="8" xr3:uid="{7179BFAD-F782-439F-BB1D-7249215D9DD8}" name="Week 7" dataDxfId="197">
       <calculatedColumnFormula>'Points calculator'!Q59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E5575ECC-2058-40E2-BD12-90C0974DB7D2}" name="Week 8" dataDxfId="194">
+    <tableColumn id="9" xr3:uid="{E5575ECC-2058-40E2-BD12-90C0974DB7D2}" name="Week 8" dataDxfId="196">
       <calculatedColumnFormula>'Points calculator'!R59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8FDE41C6-EB35-42A8-BC82-17FE917F6EED}" name="Total" dataDxfId="193">
+    <tableColumn id="10" xr3:uid="{8FDE41C6-EB35-42A8-BC82-17FE917F6EED}" name="Total" dataDxfId="195">
       <calculatedColumnFormula>SUM(N21:U21) - MIN(N21:U21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2897,11 +2911,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}" name="pointstable1" displayName="pointstable1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191" tableBorderDxfId="189" totalsRowBorderDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}" name="pointstable1" displayName="pointstable1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="194" dataDxfId="192" headerRowBorderDxfId="193" tableBorderDxfId="191" totalsRowBorderDxfId="190">
   <autoFilter ref="A1:B15" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F675884E-BFC1-4F69-B4A4-44994E445F7E}" name="Finish" dataDxfId="187"/>
-    <tableColumn id="2" xr3:uid="{81E46873-2394-4C6D-A7E0-EA300AD58D56}" name="Points" dataDxfId="186"/>
+    <tableColumn id="1" xr3:uid="{F675884E-BFC1-4F69-B4A4-44994E445F7E}" name="Finish" dataDxfId="189"/>
+    <tableColumn id="2" xr3:uid="{81E46873-2394-4C6D-A7E0-EA300AD58D56}" name="Points" dataDxfId="188"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3175,8 +3189,8 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3492,7 +3506,7 @@
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:J19"/>
+      <selection activeCell="A16" sqref="A16:V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5715,16 +5729,16 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:J15">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:J32">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V15">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21:V32">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">
@@ -5743,8 +5757,8 @@
   </sheetPr>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8626,7 +8640,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8646,7 +8660,7 @@
       <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
@@ -8895,14 +8909,15 @@
       <c r="J19" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="cHusr5jlfBAb5+kTKr/ylYv6Aic2p5S7yqpHldwZLtmfPYzilk0nol67lSRtDyFOs+ptaDC4dxmEkSFq8hgd1Q==" saltValue="EyPwTz9W/keCQBYHkP2ozQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xk0TH0+9CjiknuxCvlsCuyHMMn9LZjSWL9/+c5SHRCXs/B9kvgzCmyud85jkbuTesAd1/TcNvjpJlDTuxdujow==" saltValue="R81yi+lkIo+lXC4cnAiSpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8915,7 +8930,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8933,7 +8948,7 @@
       <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
@@ -8951,6 +8966,8 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="I2">
         <f>Roster!A4</f>
         <v>0</v>
@@ -8962,6 +8979,8 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="I3">
         <f>Roster!A5</f>
         <v>0</v>
@@ -8973,6 +8992,8 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="I4">
         <f>Roster!A6</f>
         <v>0</v>
@@ -8984,6 +9005,8 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="I5">
         <f>Roster!A7</f>
         <v>0</v>
@@ -8995,6 +9018,8 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="I6">
         <f>Roster!A8</f>
         <v>0</v>
@@ -9006,6 +9031,8 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="I7">
         <f>Roster!A9</f>
         <v>0</v>
@@ -9017,6 +9044,8 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="I8">
         <f>Roster!A10</f>
         <v>0</v>
@@ -9028,6 +9057,8 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="I9">
         <f>Roster!A11</f>
         <v>0</v>
@@ -9039,6 +9070,8 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="I10">
         <f>Roster!A12</f>
         <v>0</v>
@@ -9050,6 +9083,8 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="I11">
         <f>Roster!A13</f>
         <v>0</v>
@@ -9061,6 +9096,8 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="I12">
         <f>Roster!A14</f>
         <v>0</v>
@@ -9072,6 +9109,8 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="I13">
         <f>Roster!A15</f>
         <v>0</v>
@@ -9083,6 +9122,8 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="I14">
         <f>Roster!A16</f>
         <v>0</v>
@@ -9094,6 +9135,8 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="I15">
         <f>Roster!A17</f>
         <v>0</v>
@@ -9106,7 +9149,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="39" t="str">
         <f>Juniors!A16</f>
-        <v>Kart times pulled from: 8/12 - 8/19</v>
+        <v>Kart times pulled from: 8/18 - 8/25</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -9155,7 +9198,7 @@
       <c r="J19" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fpA3u2AQdPwj3lZNb18t5OR5lm0RzMpOvlBMLEck2jN2npCONMIiCMRZYYR9Pa9C4Gg0TRmcqCMPpxR5G3n4EQ==" saltValue="aZmqTPrlFfSAkxw/3RG7zg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="pXUta5w8iO6R1HGJUF0NaPhHuQTeltnrgB3P6F07R2emfp2fqUONdbo4g82ks8VSiNPii94x9VmkjqBRuMOrLA==" saltValue="lnisq2GiSSpATJKrdxinug==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A16:J19"/>
   </mergeCells>
@@ -9176,401 +9219,402 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J19"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.06640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53125" style="41" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="A2" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="41">
         <f>Roster!E4</f>
         <v>0</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="42">
         <f>Roster!G4</f>
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="41">
         <f>Roster!E5</f>
         <v>0</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="42">
         <f>Roster!G5</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="41">
         <f>Roster!E6</f>
         <v>0</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="42">
         <f>Roster!G6</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="41">
         <f>Roster!E7</f>
         <v>0</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="42">
         <f>Roster!G7</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="A6" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="41">
         <f>Roster!E8</f>
         <v>0</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="42">
         <f>Roster!G8</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="A7" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="41">
         <f>Roster!E9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="42">
         <f>Roster!G9</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="A8" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="41">
         <f>Roster!E10</f>
         <v>0</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="42">
         <f>Roster!G10</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="A9" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="41">
         <f>Roster!E11</f>
         <v>0</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="42">
         <f>Roster!G11</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="A10" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="41">
         <f>Roster!E12</f>
         <v>0</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="42">
         <f>Roster!G12</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="A11" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="41">
         <f>Roster!E13</f>
         <v>0</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="42">
         <f>Roster!G13</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="A12" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="41">
         <f>Roster!E14</f>
         <v>0</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="42">
         <f>Roster!G14</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="A13" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="41">
         <f>Roster!E15</f>
         <v>0</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="42">
         <f>Roster!G15</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="A14" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="41">
         <f>Roster!E16</f>
         <v>0</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="42">
         <f>Roster!G16</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="A15" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="41">
         <f>Roster!E17</f>
         <v>0</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="42">
         <f>Roster!G17</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="39" t="str">
+      <c r="A16" s="43" t="str">
         <f>Juniors!A16</f>
-        <v>Kart times pulled from: 8/12 - 8/19</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+        <v>Kart times pulled from: 8/18 - 8/25</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hyji7LmBxPCZbw3+MkCq2xgakVbVfnJ67m72aDa0ANjDZf2he1oQigTFwfHixtjSnyC0dNmuJOQQ+P7I1ndmVA==" saltValue="qqZIaafHlHDh8ekBJTFtOw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UZ7XZcoN7EbZz6YpHvj1MbhPTkbBLRSfw+wJTTxv3/Rpf3kxofPPuJsbpGXk+lO+7jfLltlJiCkvNmBYGaWY/A==" saltValue="s3/aBD59QWNS7VHV4XLXPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A16:J19"/>
   </mergeCells>
@@ -9590,403 +9634,405 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J19"/>
+      <selection activeCell="H24" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" customWidth="1"/>
-    <col min="8" max="8" width="3.265625" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.06640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.9296875" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" style="41" customWidth="1"/>
+    <col min="5" max="7" width="9.06640625" style="41"/>
+    <col min="8" max="8" width="3.265625" style="41" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="41" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="A2" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="41">
         <f>Roster!I4</f>
         <v>0</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="42">
         <f>Roster!K4</f>
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="41">
         <f>Roster!I5</f>
         <v>0</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="42">
         <f>Roster!K5</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="41">
         <f>Roster!I6</f>
         <v>0</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="42">
         <f>Roster!K6</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="41">
         <f>Roster!I7</f>
         <v>0</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="42">
         <f>Roster!K7</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="A6" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="41">
         <f>Roster!I8</f>
         <v>0</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="42">
         <f>Roster!K8</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="A7" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="41">
         <f>Roster!I9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="42">
         <f>Roster!K9</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="A8" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="41">
         <f>Roster!I10</f>
         <v>0</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="42">
         <f>Roster!K10</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="A9" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="41">
         <f>Roster!I11</f>
         <v>0</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="42">
         <f>Roster!K11</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="A10" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="41">
         <f>Roster!I12</f>
         <v>0</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="42">
         <f>Roster!K12</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="A11" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="41">
         <f>Roster!I13</f>
         <v>0</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="42">
         <f>Roster!K13</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="A12" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="41">
         <f>Roster!I14</f>
         <v>0</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="42">
         <f>Roster!K14</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="A13" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="41">
         <f>Roster!I15</f>
         <v>0</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="42">
         <f>Roster!K15</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="A14" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="41">
         <f>Roster!I16</f>
         <v>0</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="42">
         <f>Roster!K16</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="A15" s="41">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="41">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="41">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="41">
         <f>Roster!I17</f>
         <v>0</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="42">
         <f>Roster!K17</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="39" t="str">
+      <c r="A16" s="43" t="str">
         <f>Juniors!A16</f>
-        <v>Kart times pulled from: 8/12 - 8/19</v>
-      </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+        <v>Kart times pulled from: 8/18 - 8/25</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="d5G5+0UcgN/Q3C3N1SRD3405nHyLcfnQBYYVKF3abj9L52hBaWZeO9Cq1XQinw6ZpETpFcQXDUkh4gtnvreN0g==" saltValue="Vt6jN/dR+I8AlC4gCJO5gA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="w/dGAgG1ynr07thMnLfy2mKKvfIzNEnGhLMC0FXhY693TyhwDA60mc1BKRpodWkLaQ7KA+5Or/2QWmRbMNDR9Q==" saltValue="RCI2D2GU/4sU/b8AKbFwBw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A16:J19"/>
   </mergeCells>

</xml_diff>

<commit_message>
not sure what i changed lol
</commit_message>
<xml_diff>
--- a/league template.xlsx
+++ b/league template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goftaps-my.sharepoint.com/personal/sstaley_gofullthrottle_com/Documents/excel stuff/leagues/League-Points-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="703" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DDA672C-BBCB-41D5-A2FE-EE3D9CDB14BE}"/>
+  <xr:revisionPtr revIDLastSave="709" documentId="11_F25DC773A252ABDACC1048E53999438A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA9A9BD-B4DF-4397-ADD9-D2327FD3A68E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Division 2" sheetId="7" r:id="rId6"/>
     <sheet name="Division 3" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="29">
   <si>
-    <t>Name</t>
+    <t>Pro 1</t>
+  </si>
+  <si>
+    <t>Pro 2</t>
+  </si>
+  <si>
+    <t>Pro 3</t>
+  </si>
+  <si>
+    <t>Junior</t>
   </si>
   <si>
     <t>First Name</t>
@@ -54,6 +63,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Week 1</t>
@@ -83,31 +95,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Average Time</t>
-  </si>
-  <si>
-    <t>Best Time</t>
-  </si>
-  <si>
-    <t>Kart #</t>
+    <t>*Only edit points in the points calculator sheet*</t>
   </si>
   <si>
     <t>Finish</t>
   </si>
   <si>
     <t>Points</t>
-  </si>
-  <si>
-    <t>Pro 1</t>
-  </si>
-  <si>
-    <t>Pro 2</t>
-  </si>
-  <si>
-    <t>Pro 3</t>
-  </si>
-  <si>
-    <t>Junior</t>
   </si>
   <si>
     <t>Pro 1 ~~ Weekly Points Calculator</t>
@@ -122,7 +116,13 @@
     <t>Junior ~~ Weekly Points Calculator</t>
   </si>
   <si>
-    <t>*Only edit points in the points calculator sheet*</t>
+    <t>Kart #</t>
+  </si>
+  <si>
+    <t>Average Time</t>
+  </si>
+  <si>
+    <t>Best Time</t>
   </si>
   <si>
     <t>Start</t>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -562,14 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,6 +582,86 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -599,137 +671,17 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -2139,6 +2091,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2156,13 +2115,6 @@
     </dxf>
     <dxf>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2362,6 +2314,46 @@
     </dxf>
     <dxf>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2450,10 +2442,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8A66A64-948E-45A2-8B35-E39203DBCA86}" name="roster_division1" displayName="roster_division1" ref="A3:C15" totalsRowShown="0" headerRowDxfId="262" dataDxfId="261">
   <autoFilter ref="A3:C15" xr:uid="{E8A66A64-948E-45A2-8B35-E39203DBCA86}"/>
@@ -2467,130 +2455,130 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{413CA066-BE2B-49DE-9452-0AE4E5D4A4CE}" name="pointscalculator_division1" displayName="pointscalculator_division1" ref="D3:T16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="187" dataDxfId="186">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{413CA066-BE2B-49DE-9452-0AE4E5D4A4CE}" name="pointscalculator_division1" displayName="pointscalculator_division1" ref="D3:T16" headerRowCount="0" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{F54777DC-034B-4405-846B-D85CB4398F34}" name="Column1" dataDxfId="185"/>
-    <tableColumn id="2" xr3:uid="{87828A0C-FB90-4EA4-9B26-E5EA357BACC8}" name="Column2" headerRowDxfId="184" dataDxfId="183"/>
-    <tableColumn id="3" xr3:uid="{7933F018-C288-4807-985F-73CE9EFB4BBF}" name="Column3" headerRowDxfId="182" dataDxfId="181"/>
-    <tableColumn id="4" xr3:uid="{CEE14F89-D085-484E-B88A-6785163384C7}" name="Column4" headerRowDxfId="180" dataDxfId="179"/>
-    <tableColumn id="5" xr3:uid="{EDD514C2-D109-4B2F-9958-5D6E893B230D}" name="Column5" headerRowDxfId="178" dataDxfId="177"/>
-    <tableColumn id="6" xr3:uid="{11AC3DAF-2D1D-413C-A77A-2000CFA42613}" name="Column6" headerRowDxfId="176" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{1A6E6C30-0A25-43CE-8344-4A67CA14F6B6}" name="Column7" headerRowDxfId="174" dataDxfId="173"/>
-    <tableColumn id="8" xr3:uid="{71045566-6F44-4D03-ACB4-1F9B882EF703}" name="Column8" headerRowDxfId="172" dataDxfId="171"/>
-    <tableColumn id="9" xr3:uid="{EFA47D07-D6E3-437E-8FA1-A833AAF189FD}" name="Column9" headerRowDxfId="170" dataDxfId="169"/>
-    <tableColumn id="10" xr3:uid="{94A4BF73-A2A3-4928-AC13-700E2832FD15}" name="Column10" headerRowDxfId="168" dataDxfId="167"/>
-    <tableColumn id="11" xr3:uid="{9D7E6C6D-E940-4FBF-9363-95A8A6BB59CB}" name="Column11" headerRowDxfId="166" dataDxfId="165"/>
-    <tableColumn id="12" xr3:uid="{E85E09B6-3A31-4149-9FF1-4AB41A9C2E92}" name="Column12" headerRowDxfId="164" dataDxfId="163"/>
-    <tableColumn id="13" xr3:uid="{BC746882-1E84-4472-9C57-BD0D76DB39C8}" name="Column13" headerRowDxfId="162" dataDxfId="161"/>
-    <tableColumn id="14" xr3:uid="{6139B53E-4C13-45B2-8A9B-7F61D0A66175}" name="Column14" headerRowDxfId="160" dataDxfId="159"/>
-    <tableColumn id="15" xr3:uid="{E7FBC0E6-A070-48A4-9E06-7041DEC79D91}" name="Column15" headerRowDxfId="158" dataDxfId="157"/>
-    <tableColumn id="16" xr3:uid="{821CC151-5CEF-492B-824A-D2BED3D1DFEB}" name="Column16" headerRowDxfId="156" dataDxfId="155"/>
-    <tableColumn id="17" xr3:uid="{41E5B94B-F427-49FB-9779-C3AF379CFA71}" name="Column17" headerRowDxfId="154" dataDxfId="153"/>
+    <tableColumn id="1" xr3:uid="{F54777DC-034B-4405-846B-D85CB4398F34}" name="Column1" dataDxfId="181"/>
+    <tableColumn id="2" xr3:uid="{87828A0C-FB90-4EA4-9B26-E5EA357BACC8}" name="Column2" headerRowDxfId="180" dataDxfId="179"/>
+    <tableColumn id="3" xr3:uid="{7933F018-C288-4807-985F-73CE9EFB4BBF}" name="Column3" headerRowDxfId="178" dataDxfId="177"/>
+    <tableColumn id="4" xr3:uid="{CEE14F89-D085-484E-B88A-6785163384C7}" name="Column4" headerRowDxfId="176" dataDxfId="175"/>
+    <tableColumn id="5" xr3:uid="{EDD514C2-D109-4B2F-9958-5D6E893B230D}" name="Column5" headerRowDxfId="174" dataDxfId="173"/>
+    <tableColumn id="6" xr3:uid="{11AC3DAF-2D1D-413C-A77A-2000CFA42613}" name="Column6" headerRowDxfId="172" dataDxfId="171"/>
+    <tableColumn id="7" xr3:uid="{1A6E6C30-0A25-43CE-8344-4A67CA14F6B6}" name="Column7" headerRowDxfId="170" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{71045566-6F44-4D03-ACB4-1F9B882EF703}" name="Column8" headerRowDxfId="168" dataDxfId="167"/>
+    <tableColumn id="9" xr3:uid="{EFA47D07-D6E3-437E-8FA1-A833AAF189FD}" name="Column9" headerRowDxfId="166" dataDxfId="165"/>
+    <tableColumn id="10" xr3:uid="{94A4BF73-A2A3-4928-AC13-700E2832FD15}" name="Column10" headerRowDxfId="164" dataDxfId="163"/>
+    <tableColumn id="11" xr3:uid="{9D7E6C6D-E940-4FBF-9363-95A8A6BB59CB}" name="Column11" headerRowDxfId="162" dataDxfId="161"/>
+    <tableColumn id="12" xr3:uid="{E85E09B6-3A31-4149-9FF1-4AB41A9C2E92}" name="Column12" headerRowDxfId="160" dataDxfId="159"/>
+    <tableColumn id="13" xr3:uid="{BC746882-1E84-4472-9C57-BD0D76DB39C8}" name="Column13" headerRowDxfId="158" dataDxfId="157"/>
+    <tableColumn id="14" xr3:uid="{6139B53E-4C13-45B2-8A9B-7F61D0A66175}" name="Column14" headerRowDxfId="156" dataDxfId="155"/>
+    <tableColumn id="15" xr3:uid="{E7FBC0E6-A070-48A4-9E06-7041DEC79D91}" name="Column15" headerRowDxfId="154" dataDxfId="153"/>
+    <tableColumn id="16" xr3:uid="{821CC151-5CEF-492B-824A-D2BED3D1DFEB}" name="Column16" headerRowDxfId="152" dataDxfId="151"/>
+    <tableColumn id="17" xr3:uid="{41E5B94B-F427-49FB-9779-C3AF379CFA71}" name="Column17" headerRowDxfId="150" dataDxfId="149"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{CBE52FE5-F969-414E-8061-65928C310517}" name="pointscalculator_division2" displayName="pointscalculator_division2" ref="D21:T34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{CBE52FE5-F969-414E-8061-65928C310517}" name="pointscalculator_division2" displayName="pointscalculator_division2" ref="D21:T34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{A5B7E7CC-F2E9-4C49-BED9-3A47CAE54B7E}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{1F4A7765-A904-4DF6-B648-094B6BC94FBE}" name="Column2" headerRowDxfId="149" dataDxfId="148"/>
-    <tableColumn id="3" xr3:uid="{839ADCF5-8C6D-4A0C-AAB2-969A42AE8027}" name="Column3" headerRowDxfId="147" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{1731EB37-AE35-486E-855D-77128F4DDF09}" name="Column4" headerRowDxfId="145" dataDxfId="144"/>
-    <tableColumn id="5" xr3:uid="{4F3895B0-C799-4B3D-8759-283BB22EA08E}" name="Column5" headerRowDxfId="143" dataDxfId="142"/>
-    <tableColumn id="6" xr3:uid="{31207C71-AA84-443E-824A-E507F7192E3F}" name="Column6" headerRowDxfId="141" dataDxfId="140"/>
-    <tableColumn id="7" xr3:uid="{3D4AA28B-3E08-4F46-B50A-0C65CF425433}" name="Column7" headerRowDxfId="139" dataDxfId="138"/>
-    <tableColumn id="8" xr3:uid="{64223BBE-3219-453E-AD2C-61C0B9A09904}" name="Column8" headerRowDxfId="137" dataDxfId="136"/>
-    <tableColumn id="9" xr3:uid="{11687BFD-11FB-41C8-B4D4-CDB9E0136019}" name="Column9" headerRowDxfId="135" dataDxfId="134"/>
-    <tableColumn id="10" xr3:uid="{7EF49BEB-C450-4CDD-A592-0945074DF1B6}" name="Column10" headerRowDxfId="133" dataDxfId="132"/>
-    <tableColumn id="11" xr3:uid="{AAA731DE-3024-44C5-83DB-F983987C19BD}" name="Column11" headerRowDxfId="131" dataDxfId="130"/>
-    <tableColumn id="12" xr3:uid="{C2E61F83-831E-4409-9DD2-49A133F6632F}" name="Column12" headerRowDxfId="129" dataDxfId="128"/>
-    <tableColumn id="13" xr3:uid="{36F29327-806B-4BFE-98EF-D858E1BE52B2}" name="Column13" headerRowDxfId="127" dataDxfId="126"/>
-    <tableColumn id="14" xr3:uid="{BAE00B6F-FE30-4E85-AD72-BA5846AF950C}" name="Column14" headerRowDxfId="125" dataDxfId="124"/>
-    <tableColumn id="15" xr3:uid="{56476BC5-A36D-4837-8C13-38FEA912BAC5}" name="Column15" headerRowDxfId="123" dataDxfId="122"/>
-    <tableColumn id="16" xr3:uid="{1C4EAA2A-CB75-4A15-87A1-9CDC9F820B8C}" name="Column16" headerRowDxfId="121" dataDxfId="120"/>
-    <tableColumn id="17" xr3:uid="{C9171481-5E79-493E-A3D8-98929F6931FC}" name="Column17" headerRowDxfId="119" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{A5B7E7CC-F2E9-4C49-BED9-3A47CAE54B7E}" name="Column1" dataDxfId="146"/>
+    <tableColumn id="2" xr3:uid="{1F4A7765-A904-4DF6-B648-094B6BC94FBE}" name="Column2" headerRowDxfId="145" dataDxfId="144"/>
+    <tableColumn id="3" xr3:uid="{839ADCF5-8C6D-4A0C-AAB2-969A42AE8027}" name="Column3" headerRowDxfId="143" dataDxfId="142"/>
+    <tableColumn id="4" xr3:uid="{1731EB37-AE35-486E-855D-77128F4DDF09}" name="Column4" headerRowDxfId="141" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{4F3895B0-C799-4B3D-8759-283BB22EA08E}" name="Column5" headerRowDxfId="139" dataDxfId="138"/>
+    <tableColumn id="6" xr3:uid="{31207C71-AA84-443E-824A-E507F7192E3F}" name="Column6" headerRowDxfId="137" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{3D4AA28B-3E08-4F46-B50A-0C65CF425433}" name="Column7" headerRowDxfId="135" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{64223BBE-3219-453E-AD2C-61C0B9A09904}" name="Column8" headerRowDxfId="133" dataDxfId="132"/>
+    <tableColumn id="9" xr3:uid="{11687BFD-11FB-41C8-B4D4-CDB9E0136019}" name="Column9" headerRowDxfId="131" dataDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{7EF49BEB-C450-4CDD-A592-0945074DF1B6}" name="Column10" headerRowDxfId="129" dataDxfId="128"/>
+    <tableColumn id="11" xr3:uid="{AAA731DE-3024-44C5-83DB-F983987C19BD}" name="Column11" headerRowDxfId="127" dataDxfId="126"/>
+    <tableColumn id="12" xr3:uid="{C2E61F83-831E-4409-9DD2-49A133F6632F}" name="Column12" headerRowDxfId="125" dataDxfId="124"/>
+    <tableColumn id="13" xr3:uid="{36F29327-806B-4BFE-98EF-D858E1BE52B2}" name="Column13" headerRowDxfId="123" dataDxfId="122"/>
+    <tableColumn id="14" xr3:uid="{BAE00B6F-FE30-4E85-AD72-BA5846AF950C}" name="Column14" headerRowDxfId="121" dataDxfId="120"/>
+    <tableColumn id="15" xr3:uid="{56476BC5-A36D-4837-8C13-38FEA912BAC5}" name="Column15" headerRowDxfId="119" dataDxfId="118"/>
+    <tableColumn id="16" xr3:uid="{1C4EAA2A-CB75-4A15-87A1-9CDC9F820B8C}" name="Column16" headerRowDxfId="117" dataDxfId="116"/>
+    <tableColumn id="17" xr3:uid="{C9171481-5E79-493E-A3D8-98929F6931FC}" name="Column17" headerRowDxfId="115" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{29BE427D-AEEF-43FD-9197-5BC12488B6A0}" name="pointscalculator_division3" displayName="pointscalculator_division3" ref="D39:T52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{29BE427D-AEEF-43FD-9197-5BC12488B6A0}" name="pointscalculator_division3" displayName="pointscalculator_division3" ref="D39:T52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{FC4A3AA2-2C15-4A4D-A0B1-390B1DB00E83}" name="Column1" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{C31EA6F2-0FBC-4840-B86F-FF5C35E4C28C}" name="Column2" headerRowDxfId="114" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{3AFE98A5-75F5-41CB-B1EC-49E614C87BF0}" name="Column3" headerRowDxfId="112" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{48E7C085-8DFF-457A-BB2E-C6F1B98CD806}" name="Column4" headerRowDxfId="110" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{CB53D151-239B-4449-90A9-7A45D7A24982}" name="Column5" headerRowDxfId="108" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{BF1A98FD-3CA4-4E00-99CD-95C07EE77E29}" name="Column6" headerRowDxfId="106" dataDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{AAC9C9E9-A170-4DF4-A5E4-5DC08E69350B}" name="Column7" headerRowDxfId="104" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{0F098E18-2618-40F7-B7F5-A2C2726A73ED}" name="Column8" headerRowDxfId="102" dataDxfId="101"/>
-    <tableColumn id="9" xr3:uid="{DD100799-1EDD-48D5-A652-83C8A28D3E9C}" name="Column9" headerRowDxfId="100" dataDxfId="99"/>
-    <tableColumn id="10" xr3:uid="{3B30BFB9-5C90-4BEE-A4A5-25DE6F3AF3C6}" name="Column10" headerRowDxfId="98" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{8A9DB7F8-2B58-46BC-9C54-E70EB7C0A43B}" name="Column11" headerRowDxfId="96" dataDxfId="95"/>
-    <tableColumn id="12" xr3:uid="{7AF033F3-1D1E-46DB-B11A-BD277D16B337}" name="Column12" headerRowDxfId="94" dataDxfId="93"/>
-    <tableColumn id="13" xr3:uid="{ED2F8951-0A3F-41AC-B1B1-A8A039DD18BE}" name="Column13" headerRowDxfId="92" dataDxfId="91"/>
-    <tableColumn id="14" xr3:uid="{5EDC0120-BC0F-4485-80FB-2F85953C0A27}" name="Column14" headerRowDxfId="90" dataDxfId="89"/>
-    <tableColumn id="15" xr3:uid="{2F54CDE7-8BD4-4B75-A942-9CC6465B1740}" name="Column15" headerRowDxfId="88" dataDxfId="87"/>
-    <tableColumn id="16" xr3:uid="{BD867E6D-8DFD-45E7-8ED3-2FE76F68C835}" name="Column16" headerRowDxfId="86" dataDxfId="85"/>
-    <tableColumn id="17" xr3:uid="{D8E98697-97CE-4ACD-A41D-EDB9B5F2BD4E}" name="Column17" headerRowDxfId="84" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{FC4A3AA2-2C15-4A4D-A0B1-390B1DB00E83}" name="Column1" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{C31EA6F2-0FBC-4840-B86F-FF5C35E4C28C}" name="Column2" headerRowDxfId="110" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{3AFE98A5-75F5-41CB-B1EC-49E614C87BF0}" name="Column3" headerRowDxfId="108" dataDxfId="107"/>
+    <tableColumn id="4" xr3:uid="{48E7C085-8DFF-457A-BB2E-C6F1B98CD806}" name="Column4" headerRowDxfId="106" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{CB53D151-239B-4449-90A9-7A45D7A24982}" name="Column5" headerRowDxfId="104" dataDxfId="103"/>
+    <tableColumn id="6" xr3:uid="{BF1A98FD-3CA4-4E00-99CD-95C07EE77E29}" name="Column6" headerRowDxfId="102" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{AAC9C9E9-A170-4DF4-A5E4-5DC08E69350B}" name="Column7" headerRowDxfId="100" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{0F098E18-2618-40F7-B7F5-A2C2726A73ED}" name="Column8" headerRowDxfId="98" dataDxfId="97"/>
+    <tableColumn id="9" xr3:uid="{DD100799-1EDD-48D5-A652-83C8A28D3E9C}" name="Column9" headerRowDxfId="96" dataDxfId="95"/>
+    <tableColumn id="10" xr3:uid="{3B30BFB9-5C90-4BEE-A4A5-25DE6F3AF3C6}" name="Column10" headerRowDxfId="94" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{8A9DB7F8-2B58-46BC-9C54-E70EB7C0A43B}" name="Column11" headerRowDxfId="92" dataDxfId="91"/>
+    <tableColumn id="12" xr3:uid="{7AF033F3-1D1E-46DB-B11A-BD277D16B337}" name="Column12" headerRowDxfId="90" dataDxfId="89"/>
+    <tableColumn id="13" xr3:uid="{ED2F8951-0A3F-41AC-B1B1-A8A039DD18BE}" name="Column13" headerRowDxfId="88" dataDxfId="87"/>
+    <tableColumn id="14" xr3:uid="{5EDC0120-BC0F-4485-80FB-2F85953C0A27}" name="Column14" headerRowDxfId="86" dataDxfId="85"/>
+    <tableColumn id="15" xr3:uid="{2F54CDE7-8BD4-4B75-A942-9CC6465B1740}" name="Column15" headerRowDxfId="84" dataDxfId="83"/>
+    <tableColumn id="16" xr3:uid="{BD867E6D-8DFD-45E7-8ED3-2FE76F68C835}" name="Column16" headerRowDxfId="82" dataDxfId="81"/>
+    <tableColumn id="17" xr3:uid="{D8E98697-97CE-4ACD-A41D-EDB9B5F2BD4E}" name="Column17" headerRowDxfId="80" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A07179E9-6376-4F82-A951-1C094AAE9248}" name="pointscalculator_division0" displayName="pointscalculator_division0" ref="D57:T70" headerRowCount="0" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A07179E9-6376-4F82-A951-1C094AAE9248}" name="pointscalculator_division0" displayName="pointscalculator_division0" ref="D57:T70" headerRowCount="0" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E8193783-C27A-431A-9572-AFA00587EF56}" name="Column1" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{3269A5B5-EA59-431E-BF9E-6C54925FF873}" name="Column2" headerRowDxfId="79" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{D68A4479-C625-483F-8606-D5D58D70CA92}" name="Column3" headerRowDxfId="77" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{B7951688-6C6E-488C-9FCD-62063D8E1B8F}" name="Column4" headerRowDxfId="75" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{3E2FCED4-3293-4733-918D-9A21E583BB3A}" name="Column5" headerRowDxfId="73" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{BE3DF187-D34F-44CC-B9D2-6974955E38C9}" name="Column6" headerRowDxfId="71" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{5216B523-4E53-47AC-96C4-5A425B7E0549}" name="Column7" headerRowDxfId="69" dataDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{34633752-5250-4B0B-B176-38CFBA6F28C8}" name="Column8" headerRowDxfId="67" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{CE238B24-303C-4362-9B47-B981AAAE0F84}" name="Column9" headerRowDxfId="65" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{F3251511-0A59-4269-8CC5-746E6365054C}" name="Column10" headerRowDxfId="63" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{424312CA-02E5-4EC0-A003-334CC04EE9D2}" name="Column11" headerRowDxfId="61" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{0F5AC330-BD38-4A40-A538-ED741C233178}" name="Column12" headerRowDxfId="59" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{55915551-1C82-408B-80C7-E3512638D8B1}" name="Column13" headerRowDxfId="57" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{9CCB53C7-C0C9-4350-B68D-6F5E87DE5F4C}" name="Column14" headerRowDxfId="55" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{785CADF6-753C-4FE7-9311-3D5E85CAA8D0}" name="Column15" headerRowDxfId="53" dataDxfId="52"/>
-    <tableColumn id="16" xr3:uid="{EB97894A-1F48-477B-94E2-CBA9CA249DFF}" name="Column16" headerRowDxfId="51" dataDxfId="50"/>
-    <tableColumn id="17" xr3:uid="{2F00A99B-5728-43AF-A412-6250E56BA1B3}" name="Column17" headerRowDxfId="49" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{E8193783-C27A-431A-9572-AFA00587EF56}" name="Column1" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{3269A5B5-EA59-431E-BF9E-6C54925FF873}" name="Column2" headerRowDxfId="75" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{D68A4479-C625-483F-8606-D5D58D70CA92}" name="Column3" headerRowDxfId="73" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{B7951688-6C6E-488C-9FCD-62063D8E1B8F}" name="Column4" headerRowDxfId="71" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{3E2FCED4-3293-4733-918D-9A21E583BB3A}" name="Column5" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{BE3DF187-D34F-44CC-B9D2-6974955E38C9}" name="Column6" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{5216B523-4E53-47AC-96C4-5A425B7E0549}" name="Column7" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{34633752-5250-4B0B-B176-38CFBA6F28C8}" name="Column8" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{CE238B24-303C-4362-9B47-B981AAAE0F84}" name="Column9" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{F3251511-0A59-4269-8CC5-746E6365054C}" name="Column10" headerRowDxfId="59" dataDxfId="58"/>
+    <tableColumn id="11" xr3:uid="{424312CA-02E5-4EC0-A003-334CC04EE9D2}" name="Column11" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{0F5AC330-BD38-4A40-A538-ED741C233178}" name="Column12" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{55915551-1C82-408B-80C7-E3512638D8B1}" name="Column13" headerRowDxfId="53" dataDxfId="52"/>
+    <tableColumn id="14" xr3:uid="{9CCB53C7-C0C9-4350-B68D-6F5E87DE5F4C}" name="Column14" headerRowDxfId="51" dataDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{785CADF6-753C-4FE7-9311-3D5E85CAA8D0}" name="Column15" headerRowDxfId="49" dataDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{EB97894A-1F48-477B-94E2-CBA9CA249DFF}" name="Column16" headerRowDxfId="47" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{2F00A99B-5728-43AF-A412-6250E56BA1B3}" name="Column17" headerRowDxfId="45" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C066228F-627D-45C1-9355-45199E7024A2}" name="Karts_division1101223" displayName="Karts_division1101223" ref="A1:E15" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{C066228F-627D-45C1-9355-45199E7024A2}" name="Karts_division1101223" displayName="Karts_division1101223" ref="A1:E15" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{499ED437-E2A3-4DEB-9BE1-88FED55AA0D4}" name="Kart #" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{2ED3F931-9976-4869-9697-DFB0578B06A9}" name="Average Time" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{0CA1B145-AB78-4B49-B984-82824F8E6A64}" name="Best Time" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{61238CAE-31CA-4F7B-B7CA-C34249324F70}" name="Name" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{638B4A1A-D3FB-456A-8196-3FE015470B50}" name="Start" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{499ED437-E2A3-4DEB-9BE1-88FED55AA0D4}" name="Kart #" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{2ED3F931-9976-4869-9697-DFB0578B06A9}" name="Average Time" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{0CA1B145-AB78-4B49-B984-82824F8E6A64}" name="Best Time" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{61238CAE-31CA-4F7B-B7CA-C34249324F70}" name="Name" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{638B4A1A-D3FB-456A-8196-3FE015470B50}" name="Start" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{A7B10B46-A422-41FE-867F-3C32FDD82113}" name="kartpick_division1112224" displayName="kartpick_division1112224" ref="I1:J15" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{A7B10B46-A422-41FE-867F-3C32FDD82113}" name="kartpick_division1112224" displayName="kartpick_division1112224" ref="I1:J15" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A3B373D5-2CE5-4D66-8EF5-A96407FE0F68}" name="Name" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{A3B373D5-2CE5-4D66-8EF5-A96407FE0F68}" name="Name" dataDxfId="34">
       <calculatedColumnFormula>Roster!I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E06DD3EE-C704-4E82-9776-DEC1BF9920B9}" name="Weight" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{E06DD3EE-C704-4E82-9776-DEC1BF9920B9}" name="Weight" dataDxfId="33">
       <calculatedColumnFormula>Roster!K4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2599,30 +2587,30 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}" name="Karts_division1" displayName="Karts_division1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}" name="Karts_division1" displayName="Karts_division1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2F48F510-80F4-438B-9709-8408B51A9904}" name="Kart #" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B77A82F5-DEA1-428E-9E9F-7C6DD69D0486}" name="Average Time" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B07CD94E-7ED1-4DE3-8E56-A36E6E39070A}" name="Best Time" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F63BEB9B-0159-46AB-AAF5-42323633C103}" name="Name" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{85ED9692-6A48-4689-9A9B-00533CD29B14}" name="Start" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{2F48F510-80F4-438B-9709-8408B51A9904}" name="Kart #" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{B77A82F5-DEA1-428E-9E9F-7C6DD69D0486}" name="Average Time" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{B07CD94E-7ED1-4DE3-8E56-A36E6E39070A}" name="Best Time" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{F63BEB9B-0159-46AB-AAF5-42323633C103}" name="Name" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{85ED9692-6A48-4689-9A9B-00533CD29B14}" name="Start" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}" name="kartpick_division1" displayName="kartpick_division1" ref="I1:J15" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}" name="kartpick_division1" displayName="kartpick_division1" ref="I1:J15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F708E8BD-68A5-4939-B036-1CE26E2016B1}" name="Name" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{F708E8BD-68A5-4939-B036-1CE26E2016B1}" name="Name" dataDxfId="23">
       <calculatedColumnFormula>Roster!A4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B4A6FAAD-26D9-4845-ABD2-AB0AF2BF0338}" name="Weight" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{B4A6FAAD-26D9-4845-ABD2-AB0AF2BF0338}" name="Weight" dataDxfId="22">
       <calculatedColumnFormula>Roster!C4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2631,7 +2619,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5E0827B4-9E05-452D-8784-07C4744F9A8E}" name="Karts_division110" displayName="Karts_division110" ref="A1:E15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{5E0827B4-9E05-452D-8784-07C4744F9A8E}" name="Karts_division110" displayName="Karts_division110" ref="A1:E15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0B02D3BA-ECCE-428F-808D-F7CEE48D79D5}" name="Kart #" dataDxfId="19">
@@ -2651,7 +2639,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDC6AC44-B1CE-4FBC-A9AD-41D438DD98D9}" name="kartpick_division111" displayName="kartpick_division111" ref="I1:J15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDC6AC44-B1CE-4FBC-A9AD-41D438DD98D9}" name="kartpick_division111" displayName="kartpick_division111" ref="I1:J15" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
@@ -2681,36 +2669,36 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D7B5CB3-DF61-402A-8F35-D46CBBAF2AC3}" name="Karts_division11012" displayName="Karts_division11012" ref="A1:E15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6D7B5CB3-DF61-402A-8F35-D46CBBAF2AC3}" name="Karts_division11012" displayName="Karts_division11012" ref="A1:E15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:E15" xr:uid="{046D56AB-DC5D-438C-93ED-BC81A1789FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{60522C3F-A4DF-4A38-81FF-1E9B1C221E03}" name="Kart #" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{60522C3F-A4DF-4A38-81FF-1E9B1C221E03}" name="Kart #" dataDxfId="8">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Kart '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EC9933E0-4869-42D9-9C24-3AE08EEC4D7A}" name="Average Time" dataDxfId="29">
+    <tableColumn id="2" xr3:uid="{EC9933E0-4869-42D9-9C24-3AE08EEC4D7A}" name="Average Time" dataDxfId="7">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Average Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{85CAC5CF-E710-40E2-8635-6F4A05E7ECB2}" name="Best Time" dataDxfId="28">
+    <tableColumn id="3" xr3:uid="{85CAC5CF-E710-40E2-8635-6F4A05E7ECB2}" name="Best Time" dataDxfId="6">
       <calculatedColumnFormula>Karts_division1[[#This Row],[Best Time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4D4EEBB5-2C21-4DE9-B095-29000447CD26}" name="Name" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{F70CFA25-DC14-45B1-9EE0-4182384834AC}" name="Start" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{4D4EEBB5-2C21-4DE9-B095-29000447CD26}" name="Name" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{F70CFA25-DC14-45B1-9EE0-4182384834AC}" name="Start" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C94D2B82-0FF7-449F-A200-F6F1EBEDFD14}" name="kartpick_division11122" displayName="kartpick_division11122" ref="I1:J15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C94D2B82-0FF7-449F-A200-F6F1EBEDFD14}" name="kartpick_division11122" displayName="kartpick_division11122" ref="I1:J15" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="I1:J15" xr:uid="{90F4F8C9-F91B-49FF-8380-B72B9AE75D79}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:J15">
     <sortCondition descending="1" ref="J1:J15"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{268D7F68-EB66-467B-89AA-B6037DB21EFE}" name="Name" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{268D7F68-EB66-467B-89AA-B6037DB21EFE}" name="Name" dataDxfId="1">
       <calculatedColumnFormula>Roster!I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D6A8D05A-702B-41AB-BD0F-2BE11F778C3C}" name="Weight" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{D6A8D05A-702B-41AB-BD0F-2BE11F778C3C}" name="Weight" dataDxfId="0">
       <calculatedColumnFormula>Roster!K4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2743,40 +2731,40 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}" name="leaderboard_division1" displayName="leaderboard_division1" ref="A3:J15" totalsRowShown="0" headerRowDxfId="242" dataDxfId="241">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}" name="leaderboard_division1" displayName="leaderboard_division1" ref="A3:J15" totalsRowShown="0" headerRowDxfId="238" dataDxfId="237">
   <autoFilter ref="A3:J15" xr:uid="{7F01BE59-E7B1-46BE-B0E3-ACD1BE67A2FE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J15">
     <sortCondition descending="1" ref="J3:J15"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3EE385B5-186A-494C-99F2-4DA44BADE713}" name="Name" dataDxfId="240">
+    <tableColumn id="1" xr3:uid="{3EE385B5-186A-494C-99F2-4DA44BADE713}" name="Name" dataDxfId="236">
       <calculatedColumnFormula>CONCATENATE(Roster!A4, " ", Roster!B4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{05CFC75F-5D8B-4EC9-BE8F-7645475F318F}" name="Week 1" dataDxfId="239">
+    <tableColumn id="2" xr3:uid="{05CFC75F-5D8B-4EC9-BE8F-7645475F318F}" name="Week 1" dataDxfId="235">
       <calculatedColumnFormula>'Points calculator'!F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{27DA45F0-FBF3-41F0-89C5-3D9C04B59601}" name="Week 2" dataDxfId="238">
+    <tableColumn id="3" xr3:uid="{27DA45F0-FBF3-41F0-89C5-3D9C04B59601}" name="Week 2" dataDxfId="234">
       <calculatedColumnFormula>'Points calculator'!H5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1FB2A630-4026-4BD5-AB32-3BABB3917000}" name="Week 3" dataDxfId="237">
+    <tableColumn id="4" xr3:uid="{1FB2A630-4026-4BD5-AB32-3BABB3917000}" name="Week 3" dataDxfId="233">
       <calculatedColumnFormula>'Points calculator'!J5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{477B59BB-336A-42CA-B49A-D66E72883C9D}" name="Week 4" dataDxfId="236">
+    <tableColumn id="5" xr3:uid="{477B59BB-336A-42CA-B49A-D66E72883C9D}" name="Week 4" dataDxfId="232">
       <calculatedColumnFormula>'Points calculator'!K5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D41E8B54-8B08-47BE-BFC4-3D5D584C943B}" name="Week 5" dataDxfId="235">
+    <tableColumn id="6" xr3:uid="{D41E8B54-8B08-47BE-BFC4-3D5D584C943B}" name="Week 5" dataDxfId="231">
       <calculatedColumnFormula>'Points calculator'!M5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{42081221-B4AD-4019-8EBD-DDABA83F2B96}" name="Week 6" dataDxfId="234">
+    <tableColumn id="7" xr3:uid="{42081221-B4AD-4019-8EBD-DDABA83F2B96}" name="Week 6" dataDxfId="230">
       <calculatedColumnFormula>'Points calculator'!O5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{51CDE54B-C103-49F1-934C-7FB5B7C950BB}" name="Week 7" dataDxfId="233">
+    <tableColumn id="8" xr3:uid="{51CDE54B-C103-49F1-934C-7FB5B7C950BB}" name="Week 7" dataDxfId="229">
       <calculatedColumnFormula>'Points calculator'!Q5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{456B5849-E8D5-4C55-879E-90997FD8604B}" name="Week 8" dataDxfId="232">
+    <tableColumn id="9" xr3:uid="{456B5849-E8D5-4C55-879E-90997FD8604B}" name="Week 8" dataDxfId="228">
       <calculatedColumnFormula>'Points calculator'!R5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6DACC5D1-5115-470B-87C2-D8F58FFB46DE}" name="Total" dataDxfId="231">
+    <tableColumn id="10" xr3:uid="{6DACC5D1-5115-470B-87C2-D8F58FFB46DE}" name="Total" dataDxfId="227">
       <calculatedColumnFormula>SUM(B4:I4) - MIN(B4:I4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2785,40 +2773,40 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}" name="leaderboard_division2" displayName="leaderboard_division2" ref="A20:J32" totalsRowShown="0" headerRowDxfId="230" dataDxfId="229">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}" name="leaderboard_division2" displayName="leaderboard_division2" ref="A20:J32" totalsRowShown="0" headerRowDxfId="226" dataDxfId="225">
   <autoFilter ref="A20:J32" xr:uid="{4AC6C977-F2ED-4C8B-9F51-928676E5C301}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:J32">
     <sortCondition descending="1" ref="J20:J32"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8920F168-081D-48F4-B861-3BF464DCB24E}" name="Name" dataDxfId="228">
+    <tableColumn id="1" xr3:uid="{8920F168-081D-48F4-B861-3BF464DCB24E}" name="Name" dataDxfId="224">
       <calculatedColumnFormula>CONCATENATE(Roster!E4, " ", Roster!F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1FB66D7A-AD86-40F5-A827-6FD25FC3711D}" name="Week 1" dataDxfId="227">
+    <tableColumn id="2" xr3:uid="{1FB66D7A-AD86-40F5-A827-6FD25FC3711D}" name="Week 1" dataDxfId="223">
       <calculatedColumnFormula>'Points calculator'!F23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1347C6E6-6BCB-42E7-9A6C-7EEEBF3112D3}" name="Week 2" dataDxfId="226">
+    <tableColumn id="3" xr3:uid="{1347C6E6-6BCB-42E7-9A6C-7EEEBF3112D3}" name="Week 2" dataDxfId="222">
       <calculatedColumnFormula>'Points calculator'!H23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B834E847-A249-4368-BE53-6EBA45B7B65C}" name="Week 3" dataDxfId="225">
+    <tableColumn id="4" xr3:uid="{B834E847-A249-4368-BE53-6EBA45B7B65C}" name="Week 3" dataDxfId="221">
       <calculatedColumnFormula>'Points calculator'!J23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{842CDE93-7EC7-486C-AA50-AFA1DACADDE2}" name="Week 4" dataDxfId="224">
+    <tableColumn id="5" xr3:uid="{842CDE93-7EC7-486C-AA50-AFA1DACADDE2}" name="Week 4" dataDxfId="220">
       <calculatedColumnFormula>'Points calculator'!K23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0F38C0C3-9F35-46B2-B0E8-5C9089A436D9}" name="Week 5" dataDxfId="223">
+    <tableColumn id="6" xr3:uid="{0F38C0C3-9F35-46B2-B0E8-5C9089A436D9}" name="Week 5" dataDxfId="219">
       <calculatedColumnFormula>'Points calculator'!M23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E1BEDA47-31FA-4364-AD3B-6C89ED4E973E}" name="Week 6" dataDxfId="222">
+    <tableColumn id="7" xr3:uid="{E1BEDA47-31FA-4364-AD3B-6C89ED4E973E}" name="Week 6" dataDxfId="218">
       <calculatedColumnFormula>'Points calculator'!O23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8858DDC5-2FC3-484A-ABC1-8D968F1ADF71}" name="Week 7" dataDxfId="221">
+    <tableColumn id="8" xr3:uid="{8858DDC5-2FC3-484A-ABC1-8D968F1ADF71}" name="Week 7" dataDxfId="217">
       <calculatedColumnFormula>'Points calculator'!Q23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D71C639C-9F32-4C45-A01C-8AEAD864E7DB}" name="Week 8" dataDxfId="220">
+    <tableColumn id="9" xr3:uid="{D71C639C-9F32-4C45-A01C-8AEAD864E7DB}" name="Week 8" dataDxfId="216">
       <calculatedColumnFormula>'Points calculator'!R23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DA5645D4-E081-4931-84D9-D7D83BD8A055}" name="Total" dataDxfId="219">
+    <tableColumn id="10" xr3:uid="{DA5645D4-E081-4931-84D9-D7D83BD8A055}" name="Total" dataDxfId="215">
       <calculatedColumnFormula>SUM(B21:I21) - MIN(B21:I21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2827,40 +2815,40 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}" name="leaderboard_division3" displayName="leaderboard_division3" ref="M3:V15" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}" name="leaderboard_division3" displayName="leaderboard_division3" ref="M3:V15" totalsRowShown="0" headerRowDxfId="214" dataDxfId="213">
   <autoFilter ref="M3:V15" xr:uid="{07075304-D42E-4C8A-B5F9-6E003BC784DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:V15">
     <sortCondition descending="1" ref="V3:V15"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{24729B62-D12C-44C0-A782-2B723A80950C}" name="Name" dataDxfId="216">
+    <tableColumn id="1" xr3:uid="{24729B62-D12C-44C0-A782-2B723A80950C}" name="Name" dataDxfId="212">
       <calculatedColumnFormula>CONCATENATE(roster_division3[[#This Row],[First Name]], " ", roster_division3[[#This Row],[Last Name]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E2C19456-E2D6-4570-AAAC-F16C54F47CF2}" name="Week 1" dataDxfId="215">
+    <tableColumn id="2" xr3:uid="{E2C19456-E2D6-4570-AAAC-F16C54F47CF2}" name="Week 1" dataDxfId="211">
       <calculatedColumnFormula>'Points calculator'!F41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{003D5C38-C0D2-42E9-A987-6CFB7A7EB4C6}" name="Week 2" dataDxfId="214">
+    <tableColumn id="3" xr3:uid="{003D5C38-C0D2-42E9-A987-6CFB7A7EB4C6}" name="Week 2" dataDxfId="210">
       <calculatedColumnFormula>'Points calculator'!H41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AC94F960-BB0C-4A06-86A2-5ACDAFADAC89}" name="Week 3" dataDxfId="213">
+    <tableColumn id="4" xr3:uid="{AC94F960-BB0C-4A06-86A2-5ACDAFADAC89}" name="Week 3" dataDxfId="209">
       <calculatedColumnFormula>'Points calculator'!J41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F9D774A5-F6E6-4242-841D-7AF4A28B2DF0}" name="Week 4" dataDxfId="212">
+    <tableColumn id="5" xr3:uid="{F9D774A5-F6E6-4242-841D-7AF4A28B2DF0}" name="Week 4" dataDxfId="208">
       <calculatedColumnFormula>'Points calculator'!K41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EFBBCB3A-63C3-4BDD-9BE2-08298E219562}" name="Week 5" dataDxfId="211">
+    <tableColumn id="6" xr3:uid="{EFBBCB3A-63C3-4BDD-9BE2-08298E219562}" name="Week 5" dataDxfId="207">
       <calculatedColumnFormula>'Points calculator'!M41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A547CC97-7F1A-45D2-94F5-2DE2E6BEF78A}" name="Week 6" dataDxfId="210">
+    <tableColumn id="7" xr3:uid="{A547CC97-7F1A-45D2-94F5-2DE2E6BEF78A}" name="Week 6" dataDxfId="206">
       <calculatedColumnFormula>'Points calculator'!O41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5DBCD7BF-BD88-421F-99C9-3FAAE459C430}" name="Week 7" dataDxfId="209">
+    <tableColumn id="8" xr3:uid="{5DBCD7BF-BD88-421F-99C9-3FAAE459C430}" name="Week 7" dataDxfId="205">
       <calculatedColumnFormula>'Points calculator'!Q41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8054E0E9-7986-4AED-8C91-466FA9652580}" name="Week 8" dataDxfId="208">
+    <tableColumn id="9" xr3:uid="{8054E0E9-7986-4AED-8C91-466FA9652580}" name="Week 8" dataDxfId="204">
       <calculatedColumnFormula>'Points calculator'!R41</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C70C4803-97FF-4296-A9D8-829CA80E97B4}" name="Total" dataDxfId="207">
+    <tableColumn id="10" xr3:uid="{C70C4803-97FF-4296-A9D8-829CA80E97B4}" name="Total" dataDxfId="203">
       <calculatedColumnFormula>SUM(N4:U4) - MIN(N4:U4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2869,40 +2857,40 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}" name="leaderboard_division0" displayName="leaderboard_division0" ref="M20:V32" totalsRowShown="0" headerRowDxfId="206" dataDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}" name="leaderboard_division0" displayName="leaderboard_division0" ref="M20:V32" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
   <autoFilter ref="M20:V32" xr:uid="{0F30E762-B79C-466E-977F-8952D45F3546}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M21:V32">
     <sortCondition descending="1" ref="V20:V32"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F5489658-A403-4D4D-8477-63F70A31236F}" name="Name" dataDxfId="204">
+    <tableColumn id="1" xr3:uid="{F5489658-A403-4D4D-8477-63F70A31236F}" name="Name" dataDxfId="200">
       <calculatedColumnFormula>CONCATENATE(Roster!M4, " ", Roster!N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5274554A-7441-4132-9B00-0EB064D33B2E}" name="Week 1" dataDxfId="203">
+    <tableColumn id="2" xr3:uid="{5274554A-7441-4132-9B00-0EB064D33B2E}" name="Week 1" dataDxfId="199">
       <calculatedColumnFormula>'Points calculator'!F59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9575F9E7-CA68-4FE1-8BD8-120189BF05FB}" name="Week 2" dataDxfId="202">
+    <tableColumn id="3" xr3:uid="{9575F9E7-CA68-4FE1-8BD8-120189BF05FB}" name="Week 2" dataDxfId="198">
       <calculatedColumnFormula>'Points calculator'!H59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D8C8B55B-2A0D-49B7-A9AB-F098FBEE9986}" name="Week 3" dataDxfId="201">
+    <tableColumn id="4" xr3:uid="{D8C8B55B-2A0D-49B7-A9AB-F098FBEE9986}" name="Week 3" dataDxfId="197">
       <calculatedColumnFormula>'Points calculator'!J59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4ACB5F81-948D-42B6-BFFE-92CED40E0588}" name="Week 4" dataDxfId="200">
+    <tableColumn id="5" xr3:uid="{4ACB5F81-948D-42B6-BFFE-92CED40E0588}" name="Week 4" dataDxfId="196">
       <calculatedColumnFormula>'Points calculator'!K59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3554C417-4367-4989-8FD7-D5D934DE290B}" name="Week 5" dataDxfId="199">
+    <tableColumn id="6" xr3:uid="{3554C417-4367-4989-8FD7-D5D934DE290B}" name="Week 5" dataDxfId="195">
       <calculatedColumnFormula>'Points calculator'!M59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2F5C655-EB8A-4B84-8838-3144A89DFFB7}" name="Week 6" dataDxfId="198">
+    <tableColumn id="7" xr3:uid="{E2F5C655-EB8A-4B84-8838-3144A89DFFB7}" name="Week 6" dataDxfId="194">
       <calculatedColumnFormula>'Points calculator'!O59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7179BFAD-F782-439F-BB1D-7249215D9DD8}" name="Week 7" dataDxfId="197">
+    <tableColumn id="8" xr3:uid="{7179BFAD-F782-439F-BB1D-7249215D9DD8}" name="Week 7" dataDxfId="193">
       <calculatedColumnFormula>'Points calculator'!Q59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E5575ECC-2058-40E2-BD12-90C0974DB7D2}" name="Week 8" dataDxfId="196">
+    <tableColumn id="9" xr3:uid="{E5575ECC-2058-40E2-BD12-90C0974DB7D2}" name="Week 8" dataDxfId="192">
       <calculatedColumnFormula>'Points calculator'!R59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8FDE41C6-EB35-42A8-BC82-17FE917F6EED}" name="Total" dataDxfId="195">
+    <tableColumn id="10" xr3:uid="{8FDE41C6-EB35-42A8-BC82-17FE917F6EED}" name="Total" dataDxfId="191">
       <calculatedColumnFormula>SUM(N21:U21) - MIN(N21:U21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2911,11 +2899,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}" name="pointstable1" displayName="pointstable1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="194" dataDxfId="192" headerRowBorderDxfId="193" tableBorderDxfId="191" totalsRowBorderDxfId="190">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}" name="pointstable1" displayName="pointstable1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="190" dataDxfId="189" headerRowBorderDxfId="187" tableBorderDxfId="188" totalsRowBorderDxfId="186">
   <autoFilter ref="A1:B15" xr:uid="{3471E73E-F535-4BEB-BA4B-881B1409F8FD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F675884E-BFC1-4F69-B4A4-44994E445F7E}" name="Finish" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{81E46873-2394-4C6D-A7E0-EA300AD58D56}" name="Points" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{F675884E-BFC1-4F69-B4A4-44994E445F7E}" name="Finish" dataDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{81E46873-2394-4C6D-A7E0-EA300AD58D56}" name="Points" dataDxfId="184"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3189,41 +3177,41 @@
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15">
       <c r="A1" s="30" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
       <c r="E1" s="30" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F1" s="31"/>
       <c r="G1" s="31"/>
       <c r="I1" s="30" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
       <c r="M1" s="30" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -3237,45 +3225,45 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="13">
         <v>40</v>
       </c>
@@ -3289,7 +3277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15">
       <c r="C5" s="13">
         <v>0</v>
       </c>
@@ -3303,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15">
       <c r="C6" s="13">
         <v>0</v>
       </c>
@@ -3317,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15">
       <c r="C7" s="13">
         <v>0</v>
       </c>
@@ -3331,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15">
       <c r="C8" s="13">
         <v>0</v>
       </c>
@@ -3345,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15">
       <c r="C9" s="13">
         <v>0</v>
       </c>
@@ -3359,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15">
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -3373,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15">
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -3387,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15">
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -3401,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15">
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -3415,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15">
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -3429,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15">
       <c r="C15" s="13">
         <v>0</v>
       </c>
@@ -3443,40 +3431,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="9:9">
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="9:9">
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="9:9">
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="9:9">
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="9:9">
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="9:9">
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="9:9">
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="9:9">
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="9:9">
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="9:9">
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="9:9">
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="9:9">
       <c r="I28" s="13"/>
     </row>
   </sheetData>
@@ -3505,18 +3493,18 @@
   </sheetPr>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:V20"/>
+    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22">
       <c r="A1" s="32" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -3528,7 +3516,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
       <c r="M1" s="32" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
@@ -3540,7 +3528,7 @@
       <c r="U1" s="32"/>
       <c r="V1" s="32"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22">
       <c r="A2" s="32"/>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -3562,69 +3550,69 @@
       <c r="U2" s="32"/>
       <c r="V2" s="32"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="N3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="O3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="P3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="Q3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="R3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" t="s">
-        <v>8</v>
-      </c>
       <c r="S3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="T3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="U3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="str">
         <f>CONCATENATE(Roster!A4, " ", Roster!B4)</f>
         <v xml:space="preserve"> </v>
@@ -3706,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:22">
       <c r="A5" t="str">
         <f>CONCATENATE(Roster!A5, " ", Roster!B5)</f>
         <v xml:space="preserve"> </v>
@@ -3788,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22">
       <c r="A6" t="str">
         <f>CONCATENATE(Roster!A6, " ", Roster!B6)</f>
         <v xml:space="preserve"> </v>
@@ -3870,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22">
       <c r="A7" t="str">
         <f>CONCATENATE(Roster!A7, " ", Roster!B7)</f>
         <v xml:space="preserve"> </v>
@@ -3952,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22">
       <c r="A8" t="str">
         <f>CONCATENATE(Roster!A8, " ", Roster!B8)</f>
         <v xml:space="preserve"> </v>
@@ -4034,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22">
       <c r="A9" t="str">
         <f>CONCATENATE(Roster!A9, " ", Roster!B9)</f>
         <v xml:space="preserve"> </v>
@@ -4116,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22">
       <c r="A10" t="str">
         <f>CONCATENATE(Roster!A10, " ", Roster!B10)</f>
         <v xml:space="preserve"> </v>
@@ -4198,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22">
       <c r="A11" t="str">
         <f>CONCATENATE(Roster!A11, " ", Roster!B11)</f>
         <v xml:space="preserve"> </v>
@@ -4280,7 +4268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22">
       <c r="A12" t="str">
         <f>CONCATENATE(Roster!A12, " ", Roster!B12)</f>
         <v xml:space="preserve"> </v>
@@ -4362,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22">
       <c r="A13" t="str">
         <f>CONCATENATE(Roster!A13, " ", Roster!B13)</f>
         <v xml:space="preserve"> </v>
@@ -4444,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22">
       <c r="A14" t="str">
         <f>CONCATENATE(Roster!A14, " ", Roster!B14)</f>
         <v xml:space="preserve"> </v>
@@ -4526,7 +4514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22">
       <c r="A15" t="str">
         <f>CONCATENATE(Roster!A15, " ", Roster!B15)</f>
         <v xml:space="preserve"> </v>
@@ -4608,25 +4596,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22">
       <c r="I16" s="33" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J16" s="33"/>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22">
       <c r="I17" s="33"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22">
       <c r="A18" s="32" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -4638,7 +4626,7 @@
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="M18" s="32" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="N18" s="32"/>
       <c r="O18" s="32"/>
@@ -4650,7 +4638,7 @@
       <c r="U18" s="32"/>
       <c r="V18" s="32"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:22">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -4672,69 +4660,69 @@
       <c r="U19" s="32"/>
       <c r="V19" s="32"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" t="s">
         <v>7</v>
       </c>
-      <c r="F20" t="s">
+      <c r="N20" t="s">
         <v>8</v>
       </c>
-      <c r="G20" t="s">
+      <c r="O20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" t="s">
+      <c r="P20" t="s">
         <v>10</v>
       </c>
-      <c r="I20" t="s">
+      <c r="Q20" t="s">
         <v>11</v>
       </c>
-      <c r="J20" t="s">
+      <c r="R20" t="s">
         <v>12</v>
       </c>
-      <c r="M20" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" t="s">
-        <v>4</v>
-      </c>
-      <c r="O20" t="s">
-        <v>5</v>
-      </c>
-      <c r="P20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>7</v>
-      </c>
-      <c r="R20" t="s">
-        <v>8</v>
-      </c>
       <c r="S20" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="T20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="U20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="V20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="str">
         <f>CONCATENATE(Roster!E4, " ", Roster!F4)</f>
         <v xml:space="preserve"> </v>
@@ -4816,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:22">
       <c r="A22" t="str">
         <f>CONCATENATE(Roster!E5, " ", Roster!F5)</f>
         <v xml:space="preserve"> </v>
@@ -4898,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22">
       <c r="A23" t="str">
         <f>CONCATENATE(Roster!E6, " ", Roster!F6)</f>
         <v xml:space="preserve"> </v>
@@ -4980,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22">
       <c r="A24" t="str">
         <f>CONCATENATE(Roster!E7, " ", Roster!F7)</f>
         <v xml:space="preserve"> </v>
@@ -5062,7 +5050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:22">
       <c r="A25" t="str">
         <f>CONCATENATE(Roster!E8, " ", Roster!F8)</f>
         <v xml:space="preserve"> </v>
@@ -5144,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:22">
       <c r="A26" t="str">
         <f>CONCATENATE(Roster!E9, " ", Roster!F9)</f>
         <v xml:space="preserve"> </v>
@@ -5226,7 +5214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:22">
       <c r="A27" t="str">
         <f>CONCATENATE(Roster!E10, " ", Roster!F10)</f>
         <v xml:space="preserve"> </v>
@@ -5308,7 +5296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:22">
       <c r="A28" t="str">
         <f>CONCATENATE(Roster!E11, " ", Roster!F11)</f>
         <v xml:space="preserve"> </v>
@@ -5390,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:22">
       <c r="A29" t="str">
         <f>CONCATENATE(Roster!E12, " ", Roster!F12)</f>
         <v xml:space="preserve"> </v>
@@ -5472,7 +5460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:22">
       <c r="A30" t="str">
         <f>CONCATENATE(Roster!E13, " ", Roster!F13)</f>
         <v xml:space="preserve"> </v>
@@ -5554,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22">
       <c r="A31" t="str">
         <f>CONCATENATE(Roster!E14, " ", Roster!F14)</f>
         <v xml:space="preserve"> </v>
@@ -5636,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:22">
       <c r="A32" t="str">
         <f>CONCATENATE(Roster!E15, " ", Roster!F15)</f>
         <v xml:space="preserve"> </v>
@@ -5729,16 +5717,16 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:J15">
-    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:J32">
-    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4:V15">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21:V32">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">
@@ -5757,40 +5745,40 @@
   </sheetPr>
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="9.59765625" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" customWidth="1"/>
-    <col min="7" max="7" width="9.59765625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.59765625" customWidth="1"/>
-    <col min="11" max="11" width="9.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.59765625" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.59765625" customWidth="1"/>
-    <col min="15" max="15" width="10.59765625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.59765625" customWidth="1"/>
-    <col min="17" max="17" width="10.59765625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.59765625" customWidth="1"/>
-    <col min="19" max="19" width="10.59765625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.59765625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" ht="14.25" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
@@ -5809,7 +5797,7 @@
       <c r="S1" s="34"/>
       <c r="T1" s="34"/>
     </row>
-    <row r="2" spans="1:20" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:20" ht="14.65" customHeight="1" thickBot="1">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -5834,7 +5822,7 @@
       <c r="S2" s="34"/>
       <c r="T2" s="34"/>
     </row>
-    <row r="3" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:20" ht="14.65" thickBot="1">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -5842,39 +5830,39 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N3" s="23"/>
       <c r="O3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P3" s="19"/>
       <c r="Q3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="T3" s="21"/>
     </row>
-    <row r="4" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:20" ht="14.65" thickBot="1">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -5882,58 +5870,58 @@
         <v>11</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="T4" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -5985,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -6037,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -6089,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -6141,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -6193,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -6245,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -6297,7 +6285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -6349,7 +6337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -6401,7 +6389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20">
       <c r="A14" s="28">
         <v>13</v>
       </c>
@@ -6453,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>0</v>
       </c>
@@ -6505,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:20" ht="14.65" thickBot="1">
       <c r="D16" s="26" t="str">
         <f>Leaderboards!A15</f>
         <v xml:space="preserve"> </v>
@@ -6551,9 +6539,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:20" ht="14.25" customHeight="1">
       <c r="D19" s="35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
@@ -6572,7 +6560,7 @@
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
     </row>
-    <row r="20" spans="4:20" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="4:20" ht="14.65" customHeight="1" thickBot="1">
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
@@ -6591,94 +6579,94 @@
       <c r="S20" s="35"/>
       <c r="T20" s="35"/>
     </row>
-    <row r="21" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="4:20" ht="14.65" thickBot="1">
       <c r="E21" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J21" s="21"/>
       <c r="K21" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N21" s="23"/>
       <c r="O21" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R21" s="20"/>
       <c r="S21" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="T21" s="21"/>
     </row>
-    <row r="22" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="4:20" ht="14.65" thickBot="1">
       <c r="D22" s="24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R22" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="T22" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20">
       <c r="D23" s="26" t="str">
         <f>Leaderboards!A22</f>
         <v xml:space="preserve"> </v>
@@ -6724,7 +6712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:20">
       <c r="D24" s="26" t="str">
         <f>Leaderboards!A23</f>
         <v xml:space="preserve"> </v>
@@ -6770,7 +6758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:20">
       <c r="D25" s="26" t="str">
         <f>Leaderboards!A24</f>
         <v xml:space="preserve"> </v>
@@ -6816,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:20">
       <c r="D26" s="26" t="str">
         <f>Leaderboards!A25</f>
         <v xml:space="preserve"> </v>
@@ -6862,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:20">
       <c r="D27" s="26" t="str">
         <f>Leaderboards!A26</f>
         <v xml:space="preserve"> </v>
@@ -6908,7 +6896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:20">
       <c r="D28" s="26" t="str">
         <f>Leaderboards!A27</f>
         <v xml:space="preserve"> </v>
@@ -6954,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:20">
       <c r="D29" s="26" t="str">
         <f>Leaderboards!A28</f>
         <v xml:space="preserve"> </v>
@@ -7000,7 +6988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:20">
       <c r="D30" s="26" t="str">
         <f>Leaderboards!A29</f>
         <v xml:space="preserve"> </v>
@@ -7046,7 +7034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:20">
       <c r="D31" s="26" t="str">
         <f>Leaderboards!A30</f>
         <v xml:space="preserve"> </v>
@@ -7092,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:20">
       <c r="D32" s="26" t="str">
         <f>Leaderboards!A31</f>
         <v xml:space="preserve"> </v>
@@ -7138,7 +7126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:20">
       <c r="D33" s="26" t="str">
         <f>Leaderboards!A32</f>
         <v xml:space="preserve"> </v>
@@ -7184,7 +7172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="4:20" ht="14.65" thickBot="1">
       <c r="D34" s="26">
         <f>Leaderboards!A33</f>
         <v>0</v>
@@ -7230,9 +7218,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:20" ht="14.25" customHeight="1">
       <c r="D37" s="36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E37" s="36"/>
       <c r="F37" s="36"/>
@@ -7251,7 +7239,7 @@
       <c r="S37" s="36"/>
       <c r="T37" s="36"/>
     </row>
-    <row r="38" spans="4:20" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="4:20" ht="14.65" customHeight="1" thickBot="1">
       <c r="D38" s="36"/>
       <c r="E38" s="36"/>
       <c r="F38" s="36"/>
@@ -7270,94 +7258,94 @@
       <c r="S38" s="36"/>
       <c r="T38" s="36"/>
     </row>
-    <row r="39" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="4:20" ht="14.65" thickBot="1">
       <c r="E39" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H39" s="20"/>
       <c r="I39" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J39" s="21"/>
       <c r="K39" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L39" s="22"/>
       <c r="M39" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N39" s="23"/>
       <c r="O39" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P39" s="19"/>
       <c r="Q39" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R39" s="20"/>
       <c r="S39" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="T39" s="21"/>
     </row>
-    <row r="40" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="4:20" ht="14.65" thickBot="1">
       <c r="D40" s="24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R40" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="T40" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="4:20" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="4:20">
       <c r="D41" s="26" t="str">
         <f>Leaderboards!M4</f>
         <v xml:space="preserve"> </v>
@@ -7403,7 +7391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:20">
       <c r="D42" s="26" t="str">
         <f>Leaderboards!M5</f>
         <v xml:space="preserve"> </v>
@@ -7449,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:20">
       <c r="D43" s="26" t="str">
         <f>Leaderboards!M6</f>
         <v xml:space="preserve"> </v>
@@ -7495,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:20">
       <c r="D44" s="26" t="str">
         <f>Leaderboards!M7</f>
         <v xml:space="preserve"> </v>
@@ -7541,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:20">
       <c r="D45" s="26" t="str">
         <f>Leaderboards!M8</f>
         <v xml:space="preserve"> </v>
@@ -7587,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:20">
       <c r="D46" s="26" t="str">
         <f>Leaderboards!M9</f>
         <v xml:space="preserve"> </v>
@@ -7633,7 +7621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:20">
       <c r="D47" s="26" t="str">
         <f>Leaderboards!M10</f>
         <v xml:space="preserve"> </v>
@@ -7679,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:20">
       <c r="D48" s="26" t="str">
         <f>Leaderboards!M11</f>
         <v xml:space="preserve"> </v>
@@ -7725,7 +7713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:20">
       <c r="D49" s="26" t="str">
         <f>Leaderboards!M12</f>
         <v xml:space="preserve"> </v>
@@ -7771,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:20">
       <c r="D50" s="26" t="str">
         <f>Leaderboards!M13</f>
         <v xml:space="preserve"> </v>
@@ -7817,7 +7805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:20">
       <c r="D51" s="26" t="str">
         <f>Leaderboards!M14</f>
         <v xml:space="preserve"> </v>
@@ -7863,7 +7851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="4:20" ht="14.65" thickBot="1">
       <c r="D52" s="26" t="str">
         <f>Leaderboards!M15</f>
         <v xml:space="preserve"> </v>
@@ -7909,9 +7897,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="4:20" ht="14.25" customHeight="1">
       <c r="D55" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E55" s="37"/>
       <c r="F55" s="37"/>
@@ -7930,7 +7918,7 @@
       <c r="S55" s="37"/>
       <c r="T55" s="37"/>
     </row>
-    <row r="56" spans="4:20" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="4:20" ht="14.65" customHeight="1" thickBot="1">
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
@@ -7949,94 +7937,94 @@
       <c r="S56" s="37"/>
       <c r="T56" s="37"/>
     </row>
-    <row r="57" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="4:20" ht="14.65" thickBot="1">
       <c r="E57" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F57" s="19"/>
       <c r="G57" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J57" s="21"/>
       <c r="K57" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L57" s="22"/>
       <c r="M57" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N57" s="23"/>
       <c r="O57" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P57" s="19"/>
       <c r="Q57" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R57" s="20"/>
       <c r="S57" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="T57" s="21"/>
     </row>
-    <row r="58" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="4:20" ht="14.65" thickBot="1">
       <c r="D58" s="24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R58" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S58" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="T58" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="4:20" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="4:20">
       <c r="D59" s="26" t="str">
         <f>Leaderboards!M21</f>
         <v xml:space="preserve"> </v>
@@ -8082,7 +8070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="60" spans="4:20">
       <c r="D60" s="26" t="str">
         <f>Leaderboards!M22</f>
         <v xml:space="preserve"> </v>
@@ -8128,7 +8116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="61" spans="4:20">
       <c r="D61" s="26" t="str">
         <f>Leaderboards!M23</f>
         <v xml:space="preserve"> </v>
@@ -8174,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="62" spans="4:20">
       <c r="D62" s="26" t="str">
         <f>Leaderboards!M24</f>
         <v xml:space="preserve"> </v>
@@ -8220,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="63" spans="4:20">
       <c r="D63" s="26" t="str">
         <f>Leaderboards!M25</f>
         <v xml:space="preserve"> </v>
@@ -8266,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="64" spans="4:20">
       <c r="D64" s="26" t="str">
         <f>Leaderboards!M26</f>
         <v xml:space="preserve"> </v>
@@ -8312,7 +8300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="65" spans="4:20">
       <c r="D65" s="26" t="str">
         <f>Leaderboards!M27</f>
         <v xml:space="preserve"> </v>
@@ -8358,7 +8346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="66" spans="4:20">
       <c r="D66" s="26" t="str">
         <f>Leaderboards!M28</f>
         <v xml:space="preserve"> </v>
@@ -8404,7 +8392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="67" spans="4:20">
       <c r="D67" s="26" t="str">
         <f>Leaderboards!M29</f>
         <v xml:space="preserve"> </v>
@@ -8450,7 +8438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="68" spans="4:20">
       <c r="D68" s="26" t="str">
         <f>Leaderboards!M30</f>
         <v xml:space="preserve"> </v>
@@ -8496,7 +8484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="4:20" x14ac:dyDescent="0.45">
+    <row r="69" spans="4:20">
       <c r="D69" s="26" t="str">
         <f>Leaderboards!M31</f>
         <v xml:space="preserve"> </v>
@@ -8542,7 +8530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="4:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="4:20" ht="14.65" thickBot="1">
       <c r="D70" s="26" t="str">
         <f>Leaderboards!M32</f>
         <v xml:space="preserve"> </v>
@@ -8643,40 +8631,40 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" customWidth="1"/>
-    <col min="8" max="8" width="3.265625" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -8689,7 +8677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -8702,7 +8690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -8715,7 +8703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -8728,7 +8716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -8741,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -8754,7 +8742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -8767,7 +8755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -8780,7 +8768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -8793,7 +8781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -8806,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -8819,7 +8807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -8832,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -8845,7 +8833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -8858,7 +8846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16" s="38" t="s">
         <v>28</v>
       </c>
@@ -8872,7 +8860,7 @@
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10">
       <c r="A17" s="31"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -8884,7 +8872,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" s="31"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -8896,7 +8884,7 @@
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" s="31"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
@@ -8929,44 +8917,48 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="I2">
         <f>Roster!A4</f>
@@ -8977,7 +8969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -8990,7 +8982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -9003,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -9016,7 +9008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -9029,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -9042,7 +9034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -9055,7 +9047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -9068,7 +9060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -9081,7 +9073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -9094,7 +9086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -9107,7 +9099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -9120,7 +9112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -9133,7 +9125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -9146,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16" s="39" t="str">
         <f>Juniors!A16</f>
         <v>Kart times pulled from: 8/18 - 8/25</v>
@@ -9161,7 +9153,7 @@
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10">
       <c r="A17" s="40"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
@@ -9173,7 +9165,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" s="40"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
@@ -9185,7 +9177,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -9222,396 +9214,395 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53125" style="41" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="41"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="41" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2">
         <f>Roster!E4</f>
         <v>0</v>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="14">
         <f>Roster!G4</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="41">
+    <row r="3" spans="1:10">
+      <c r="A3">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I3" s="41">
+      <c r="I3">
         <f>Roster!E5</f>
         <v>0</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="14">
         <f>Roster!G5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="41">
+    <row r="4" spans="1:10">
+      <c r="A4">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4">
         <f>Roster!E6</f>
         <v>0</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="14">
         <f>Roster!G6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="41">
+    <row r="5" spans="1:10">
+      <c r="A5">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5">
         <f>Roster!E7</f>
         <v>0</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="14">
         <f>Roster!G7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="41">
+    <row r="6" spans="1:10">
+      <c r="A6">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6">
         <f>Roster!E8</f>
         <v>0</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="14">
         <f>Roster!G8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="41">
+    <row r="7" spans="1:10">
+      <c r="A7">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I7" s="41">
+      <c r="I7">
         <f>Roster!E9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="14">
         <f>Roster!G9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="41">
+    <row r="8" spans="1:10">
+      <c r="A8">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8">
         <f>Roster!E10</f>
         <v>0</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="14">
         <f>Roster!G10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="41">
+    <row r="9" spans="1:10">
+      <c r="A9">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9">
         <f>Roster!E11</f>
         <v>0</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="14">
         <f>Roster!G11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="41">
+    <row r="10" spans="1:10">
+      <c r="A10">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10">
         <f>Roster!E12</f>
         <v>0</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="14">
         <f>Roster!G12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="41">
+    <row r="11" spans="1:10">
+      <c r="A11">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11">
         <f>Roster!E13</f>
         <v>0</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="14">
         <f>Roster!G13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="41">
+    <row r="12" spans="1:10">
+      <c r="A12">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I12" s="41">
+      <c r="I12">
         <f>Roster!E14</f>
         <v>0</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="14">
         <f>Roster!G14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="41">
+    <row r="13" spans="1:10">
+      <c r="A13">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13">
         <f>Roster!E15</f>
         <v>0</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="14">
         <f>Roster!G15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="41">
+    <row r="14" spans="1:10">
+      <c r="A14">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I14" s="41">
+      <c r="I14">
         <f>Roster!E16</f>
         <v>0</v>
       </c>
-      <c r="J14" s="42">
+      <c r="J14" s="14">
         <f>Roster!G16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="41">
+    <row r="15" spans="1:10">
+      <c r="A15">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I15" s="41">
+      <c r="I15">
         <f>Roster!E17</f>
         <v>0</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="14">
         <f>Roster!G17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="43" t="str">
+    <row r="16" spans="1:10">
+      <c r="A16" s="39" t="str">
         <f>Juniors!A16</f>
         <v>Kart times pulled from: 8/18 - 8/25</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="UZ7XZcoN7EbZz6YpHvj1MbhPTkbBLRSfw+wJTTxv3/Rpf3kxofPPuJsbpGXk+lO+7jfLltlJiCkvNmBYGaWY/A==" saltValue="s3/aBD59QWNS7VHV4XLXPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -9634,402 +9625,400 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="A1:XFD1048576"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.06640625" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" style="41" customWidth="1"/>
-    <col min="5" max="7" width="9.06640625" style="41"/>
-    <col min="8" max="8" width="3.265625" style="41" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="41" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="41"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="41" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="41">
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I2" s="41">
+      <c r="I2">
         <f>Roster!I4</f>
         <v>0</v>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="14">
         <f>Roster!K4</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="41">
+    <row r="3" spans="1:10">
+      <c r="A3">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I3" s="41">
+      <c r="I3">
         <f>Roster!I5</f>
         <v>0</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="14">
         <f>Roster!K5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="41">
+    <row r="4" spans="1:10">
+      <c r="A4">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4">
         <f>Roster!I6</f>
         <v>0</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="14">
         <f>Roster!K6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="41">
+    <row r="5" spans="1:10">
+      <c r="A5">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5">
         <f>Roster!I7</f>
         <v>0</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="14">
         <f>Roster!K7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="41">
+    <row r="6" spans="1:10">
+      <c r="A6">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6">
         <f>Roster!I8</f>
         <v>0</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="14">
         <f>Roster!K8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="41">
+    <row r="7" spans="1:10">
+      <c r="A7">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I7" s="41">
+      <c r="I7">
         <f>Roster!I9</f>
         <v>0</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="14">
         <f>Roster!K9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="41">
+    <row r="8" spans="1:10">
+      <c r="A8">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8">
         <f>Roster!I10</f>
         <v>0</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="14">
         <f>Roster!K10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="41">
+    <row r="9" spans="1:10">
+      <c r="A9">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9">
         <f>Roster!I11</f>
         <v>0</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="14">
         <f>Roster!K11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="41">
+    <row r="10" spans="1:10">
+      <c r="A10">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10">
         <f>Roster!I12</f>
         <v>0</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="14">
         <f>Roster!K12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="41">
+    <row r="11" spans="1:10">
+      <c r="A11">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11">
         <f>Roster!I13</f>
         <v>0</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="14">
         <f>Roster!K13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="41">
+    <row r="12" spans="1:10">
+      <c r="A12">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I12" s="41">
+      <c r="I12">
         <f>Roster!I14</f>
         <v>0</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="14">
         <f>Roster!K14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="41">
+    <row r="13" spans="1:10">
+      <c r="A13">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13">
         <f>Roster!I15</f>
         <v>0</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="14">
         <f>Roster!K15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="41">
+    <row r="14" spans="1:10">
+      <c r="A14">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I14" s="41">
+      <c r="I14">
         <f>Roster!I16</f>
         <v>0</v>
       </c>
-      <c r="J14" s="42">
+      <c r="J14" s="14">
         <f>Roster!K16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="41">
+    <row r="15" spans="1:10">
+      <c r="A15">
         <f>Karts_division1[[#This Row],[Kart '#]]</f>
         <v>0</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15">
         <f>Karts_division1[[#This Row],[Average Time]]</f>
         <v>0</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15">
         <f>Karts_division1[[#This Row],[Best Time]]</f>
         <v>0</v>
       </c>
-      <c r="I15" s="41">
+      <c r="I15">
         <f>Roster!I17</f>
         <v>0</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="14">
         <f>Roster!K17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="43" t="str">
+    <row r="16" spans="1:10">
+      <c r="A16" s="39" t="str">
         <f>Juniors!A16</f>
         <v>Kart times pulled from: 8/18 - 8/25</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="w/dGAgG1ynr07thMnLfy2mKKvfIzNEnGhLMC0FXhY693TyhwDA60mc1BKRpodWkLaQ7KA+5Or/2QWmRbMNDR9Q==" saltValue="RCI2D2GU/4sU/b8AKbFwBw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>